<commit_message>
adiciona a tabela tbl_sobre_empresa e o campo ativo na tbl_imagem_veiculo_parceiro
</commit_message>
<xml_diff>
--- a/database/dicionario/dicionario_de_dados.xltx.xlsx
+++ b/database/dicionario/dicionario_de_dados.xltx.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.107.144.10\portalautocenter\database\dicionario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\site\Portal-Auto-Center\database\dicionario\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0587AB0F-54A6-4CC0-8827-E23E64C0DCAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dicionario_de_dados" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="264">
   <si>
     <t>id_cliente</t>
   </si>
@@ -780,9 +781,6 @@
     <t>SIM</t>
   </si>
   <si>
-    <t>NÃO</t>
-  </si>
-  <si>
     <t>valor_abastecimento</t>
   </si>
   <si>
@@ -799,12 +797,27 @@
   </si>
   <si>
     <t>log_controle_abastecimento</t>
+  </si>
+  <si>
+    <t>Tabela: tbl_sobre_empresa-</t>
+  </si>
+  <si>
+    <t>id_sobre_empresa</t>
+  </si>
+  <si>
+    <t>VARCHAR(480)</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>VARCHAR(2800)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1417,7 +1430,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1438,6 +1451,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1456,32 +1497,11 @@
     <xf numFmtId="0" fontId="13" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1515,10 +1535,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1838,11 +1858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G448"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G460"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A427" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I447" sqref="I447"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,26 +1877,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2120,26 +2140,26 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2231,26 +2251,26 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -2441,26 +2461,26 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="10"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="20"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -2685,26 +2705,26 @@
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="10"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -2777,26 +2797,26 @@
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="10"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="17"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
@@ -2869,26 +2889,26 @@
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="10"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="20"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
@@ -3075,26 +3095,26 @@
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="10"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="20"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="17"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
@@ -3167,26 +3187,26 @@
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="10"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="20"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="17"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
@@ -3339,26 +3359,26 @@
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="10"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="20"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="17"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
@@ -3663,26 +3683,26 @@
       <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B107" s="9"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="10"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="20"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="14" t="s">
+      <c r="A108" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="15"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
-      <c r="F108" s="15"/>
-      <c r="G108" s="16"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
@@ -3755,26 +3775,26 @@
       <c r="G112" s="2"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="B113" s="9"/>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="9"/>
-      <c r="G113" s="10"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="20"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="14" t="s">
+      <c r="A114" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="15"/>
-      <c r="F114" s="15"/>
-      <c r="G114" s="16"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="17"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
@@ -3925,26 +3945,26 @@
       <c r="G122" s="2"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
+      <c r="A123" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="B123" s="9"/>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
-      <c r="G123" s="10"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+      <c r="G123" s="20"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="14" t="s">
+      <c r="A124" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B124" s="15"/>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="15"/>
-      <c r="G124" s="16"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="17"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
@@ -4017,26 +4037,26 @@
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
+      <c r="A129" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="B129" s="9"/>
-      <c r="C129" s="9"/>
-      <c r="D129" s="9"/>
-      <c r="E129" s="9"/>
-      <c r="F129" s="9"/>
-      <c r="G129" s="10"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+      <c r="G129" s="20"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="14" t="s">
+      <c r="A130" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B130" s="15"/>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
-      <c r="E130" s="15"/>
-      <c r="F130" s="15"/>
-      <c r="G130" s="16"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="17"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
@@ -4128,26 +4148,26 @@
       <c r="G135" s="2"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
+      <c r="A136" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B136" s="9"/>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9"/>
-      <c r="E136" s="9"/>
-      <c r="F136" s="9"/>
-      <c r="G136" s="10"/>
+      <c r="B136" s="19"/>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="20"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="14" t="s">
+      <c r="A137" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B137" s="15"/>
-      <c r="C137" s="15"/>
-      <c r="D137" s="15"/>
-      <c r="E137" s="15"/>
-      <c r="F137" s="15"/>
-      <c r="G137" s="16"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="16"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="17"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
@@ -4279,26 +4299,26 @@
       <c r="G144" s="2"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="8" t="s">
+      <c r="A145" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="B145" s="9"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
-      <c r="E145" s="9"/>
-      <c r="F145" s="9"/>
-      <c r="G145" s="10"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="19"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="19"/>
+      <c r="G145" s="20"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="14" t="s">
+      <c r="A146" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B146" s="15"/>
-      <c r="C146" s="15"/>
-      <c r="D146" s="15"/>
-      <c r="E146" s="15"/>
-      <c r="F146" s="15"/>
-      <c r="G146" s="16"/>
+      <c r="B146" s="16"/>
+      <c r="C146" s="16"/>
+      <c r="D146" s="16"/>
+      <c r="E146" s="16"/>
+      <c r="F146" s="16"/>
+      <c r="G146" s="17"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
@@ -4371,26 +4391,26 @@
       <c r="G150" s="2"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
+      <c r="A151" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="9"/>
-      <c r="F151" s="9"/>
-      <c r="G151" s="10"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="19"/>
+      <c r="D151" s="19"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="19"/>
+      <c r="G151" s="20"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="14" t="s">
+      <c r="A152" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B152" s="15"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="15"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="15"/>
-      <c r="G152" s="16"/>
+      <c r="B152" s="16"/>
+      <c r="C152" s="16"/>
+      <c r="D152" s="16"/>
+      <c r="E152" s="16"/>
+      <c r="F152" s="16"/>
+      <c r="G152" s="17"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
@@ -4503,26 +4523,26 @@
       <c r="G158" s="2"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="8" t="s">
+      <c r="A159" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="B159" s="9"/>
-      <c r="C159" s="9"/>
-      <c r="D159" s="9"/>
-      <c r="E159" s="9"/>
-      <c r="F159" s="9"/>
-      <c r="G159" s="10"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="19"/>
+      <c r="G159" s="20"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="14" t="s">
+      <c r="A160" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B160" s="15"/>
-      <c r="C160" s="15"/>
-      <c r="D160" s="15"/>
-      <c r="E160" s="15"/>
-      <c r="F160" s="15"/>
-      <c r="G160" s="16"/>
+      <c r="B160" s="16"/>
+      <c r="C160" s="16"/>
+      <c r="D160" s="16"/>
+      <c r="E160" s="16"/>
+      <c r="F160" s="16"/>
+      <c r="G160" s="17"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
@@ -4614,26 +4634,26 @@
       <c r="G165" s="2"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="8" t="s">
+      <c r="A166" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="B166" s="9"/>
-      <c r="C166" s="9"/>
-      <c r="D166" s="9"/>
-      <c r="E166" s="9"/>
-      <c r="F166" s="9"/>
-      <c r="G166" s="10"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="19"/>
+      <c r="D166" s="19"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="19"/>
+      <c r="G166" s="20"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="14" t="s">
+      <c r="A167" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B167" s="15"/>
-      <c r="C167" s="15"/>
-      <c r="D167" s="15"/>
-      <c r="E167" s="15"/>
-      <c r="F167" s="15"/>
-      <c r="G167" s="16"/>
+      <c r="B167" s="16"/>
+      <c r="C167" s="16"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="16"/>
+      <c r="G167" s="17"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
@@ -4706,26 +4726,26 @@
       <c r="G171" s="2"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="8" t="s">
+      <c r="A172" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="B172" s="9"/>
-      <c r="C172" s="9"/>
-      <c r="D172" s="9"/>
-      <c r="E172" s="9"/>
-      <c r="F172" s="9"/>
-      <c r="G172" s="10"/>
+      <c r="B172" s="19"/>
+      <c r="C172" s="19"/>
+      <c r="D172" s="19"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="19"/>
+      <c r="G172" s="20"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="14" t="s">
+      <c r="A173" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B173" s="15"/>
-      <c r="C173" s="15"/>
-      <c r="D173" s="15"/>
-      <c r="E173" s="15"/>
-      <c r="F173" s="15"/>
-      <c r="G173" s="16"/>
+      <c r="B173" s="16"/>
+      <c r="C173" s="16"/>
+      <c r="D173" s="16"/>
+      <c r="E173" s="16"/>
+      <c r="F173" s="16"/>
+      <c r="G173" s="17"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
@@ -4817,26 +4837,26 @@
       <c r="G178" s="2"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="8" t="s">
+      <c r="A179" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B179" s="9"/>
-      <c r="C179" s="9"/>
-      <c r="D179" s="9"/>
-      <c r="E179" s="9"/>
-      <c r="F179" s="9"/>
-      <c r="G179" s="10"/>
+      <c r="B179" s="19"/>
+      <c r="C179" s="19"/>
+      <c r="D179" s="19"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="19"/>
+      <c r="G179" s="20"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="14" t="s">
+      <c r="A180" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B180" s="15"/>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
-      <c r="G180" s="16"/>
+      <c r="B180" s="16"/>
+      <c r="C180" s="16"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="16"/>
+      <c r="F180" s="16"/>
+      <c r="G180" s="17"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
@@ -4928,26 +4948,26 @@
       <c r="G185" s="2"/>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="8" t="s">
+      <c r="A186" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="B186" s="9"/>
-      <c r="C186" s="9"/>
-      <c r="D186" s="9"/>
-      <c r="E186" s="9"/>
-      <c r="F186" s="9"/>
-      <c r="G186" s="10"/>
+      <c r="B186" s="19"/>
+      <c r="C186" s="19"/>
+      <c r="D186" s="19"/>
+      <c r="E186" s="19"/>
+      <c r="F186" s="19"/>
+      <c r="G186" s="20"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="14" t="s">
+      <c r="A187" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B187" s="15"/>
-      <c r="C187" s="15"/>
-      <c r="D187" s="15"/>
-      <c r="E187" s="15"/>
-      <c r="F187" s="15"/>
-      <c r="G187" s="16"/>
+      <c r="B187" s="16"/>
+      <c r="C187" s="16"/>
+      <c r="D187" s="16"/>
+      <c r="E187" s="16"/>
+      <c r="F187" s="16"/>
+      <c r="G187" s="17"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
@@ -5020,26 +5040,26 @@
       <c r="G191" s="2"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="8" t="s">
+      <c r="A192" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B192" s="9"/>
-      <c r="C192" s="9"/>
-      <c r="D192" s="9"/>
-      <c r="E192" s="9"/>
-      <c r="F192" s="9"/>
-      <c r="G192" s="10"/>
+      <c r="B192" s="19"/>
+      <c r="C192" s="19"/>
+      <c r="D192" s="19"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="19"/>
+      <c r="G192" s="20"/>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" s="14" t="s">
+      <c r="A193" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B193" s="15"/>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-      <c r="E193" s="15"/>
-      <c r="F193" s="15"/>
-      <c r="G193" s="16"/>
+      <c r="B193" s="16"/>
+      <c r="C193" s="16"/>
+      <c r="D193" s="16"/>
+      <c r="E193" s="16"/>
+      <c r="F193" s="16"/>
+      <c r="G193" s="17"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
@@ -5112,26 +5132,26 @@
       <c r="G197" s="2"/>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A198" s="8" t="s">
+      <c r="A198" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="B198" s="9"/>
-      <c r="C198" s="9"/>
-      <c r="D198" s="9"/>
-      <c r="E198" s="9"/>
-      <c r="F198" s="9"/>
-      <c r="G198" s="10"/>
+      <c r="B198" s="19"/>
+      <c r="C198" s="19"/>
+      <c r="D198" s="19"/>
+      <c r="E198" s="19"/>
+      <c r="F198" s="19"/>
+      <c r="G198" s="20"/>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="14" t="s">
+      <c r="A199" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B199" s="15"/>
-      <c r="C199" s="15"/>
-      <c r="D199" s="15"/>
-      <c r="E199" s="15"/>
-      <c r="F199" s="15"/>
-      <c r="G199" s="16"/>
+      <c r="B199" s="16"/>
+      <c r="C199" s="16"/>
+      <c r="D199" s="16"/>
+      <c r="E199" s="16"/>
+      <c r="F199" s="16"/>
+      <c r="G199" s="17"/>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
@@ -5223,26 +5243,26 @@
       <c r="G204" s="2"/>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A205" s="8" t="s">
+      <c r="A205" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="B205" s="9"/>
-      <c r="C205" s="9"/>
-      <c r="D205" s="9"/>
-      <c r="E205" s="9"/>
-      <c r="F205" s="9"/>
-      <c r="G205" s="10"/>
+      <c r="B205" s="19"/>
+      <c r="C205" s="19"/>
+      <c r="D205" s="19"/>
+      <c r="E205" s="19"/>
+      <c r="F205" s="19"/>
+      <c r="G205" s="20"/>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A206" s="14" t="s">
+      <c r="A206" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B206" s="15"/>
-      <c r="C206" s="15"/>
-      <c r="D206" s="15"/>
-      <c r="E206" s="15"/>
-      <c r="F206" s="15"/>
-      <c r="G206" s="16"/>
+      <c r="B206" s="16"/>
+      <c r="C206" s="16"/>
+      <c r="D206" s="16"/>
+      <c r="E206" s="16"/>
+      <c r="F206" s="16"/>
+      <c r="G206" s="17"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
@@ -5488,26 +5508,26 @@
       <c r="G219" s="2"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="8" t="s">
+      <c r="A220" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B220" s="9"/>
-      <c r="C220" s="9"/>
-      <c r="D220" s="9"/>
-      <c r="E220" s="9"/>
-      <c r="F220" s="9"/>
-      <c r="G220" s="10"/>
+      <c r="B220" s="19"/>
+      <c r="C220" s="19"/>
+      <c r="D220" s="19"/>
+      <c r="E220" s="19"/>
+      <c r="F220" s="19"/>
+      <c r="G220" s="20"/>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A221" s="14" t="s">
+      <c r="A221" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B221" s="15"/>
-      <c r="C221" s="15"/>
-      <c r="D221" s="15"/>
-      <c r="E221" s="15"/>
-      <c r="F221" s="15"/>
-      <c r="G221" s="16"/>
+      <c r="B221" s="16"/>
+      <c r="C221" s="16"/>
+      <c r="D221" s="16"/>
+      <c r="E221" s="16"/>
+      <c r="F221" s="16"/>
+      <c r="G221" s="17"/>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
@@ -5656,26 +5676,26 @@
       <c r="G229" s="2"/>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="8" t="s">
+      <c r="A230" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="B230" s="9"/>
-      <c r="C230" s="9"/>
-      <c r="D230" s="9"/>
-      <c r="E230" s="9"/>
-      <c r="F230" s="9"/>
-      <c r="G230" s="10"/>
+      <c r="B230" s="19"/>
+      <c r="C230" s="19"/>
+      <c r="D230" s="19"/>
+      <c r="E230" s="19"/>
+      <c r="F230" s="19"/>
+      <c r="G230" s="20"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="14" t="s">
+      <c r="A231" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B231" s="15"/>
-      <c r="C231" s="15"/>
-      <c r="D231" s="15"/>
-      <c r="E231" s="15"/>
-      <c r="F231" s="15"/>
-      <c r="G231" s="16"/>
+      <c r="B231" s="16"/>
+      <c r="C231" s="16"/>
+      <c r="D231" s="16"/>
+      <c r="E231" s="16"/>
+      <c r="F231" s="16"/>
+      <c r="G231" s="17"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
@@ -5748,26 +5768,26 @@
       <c r="G235" s="2"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="8" t="s">
+      <c r="A236" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B236" s="9"/>
-      <c r="C236" s="9"/>
-      <c r="D236" s="9"/>
-      <c r="E236" s="9"/>
-      <c r="F236" s="9"/>
-      <c r="G236" s="10"/>
+      <c r="B236" s="19"/>
+      <c r="C236" s="19"/>
+      <c r="D236" s="19"/>
+      <c r="E236" s="19"/>
+      <c r="F236" s="19"/>
+      <c r="G236" s="20"/>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A237" s="14" t="s">
+      <c r="A237" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B237" s="15"/>
-      <c r="C237" s="15"/>
-      <c r="D237" s="15"/>
-      <c r="E237" s="15"/>
-      <c r="F237" s="15"/>
-      <c r="G237" s="16"/>
+      <c r="B237" s="16"/>
+      <c r="C237" s="16"/>
+      <c r="D237" s="16"/>
+      <c r="E237" s="16"/>
+      <c r="F237" s="16"/>
+      <c r="G237" s="17"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
@@ -5859,26 +5879,26 @@
       <c r="G242" s="2"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243" s="8" t="s">
+      <c r="A243" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="B243" s="9"/>
-      <c r="C243" s="9"/>
-      <c r="D243" s="9"/>
-      <c r="E243" s="9"/>
-      <c r="F243" s="9"/>
-      <c r="G243" s="10"/>
+      <c r="B243" s="19"/>
+      <c r="C243" s="19"/>
+      <c r="D243" s="19"/>
+      <c r="E243" s="19"/>
+      <c r="F243" s="19"/>
+      <c r="G243" s="20"/>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="14" t="s">
+      <c r="A244" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B244" s="15"/>
-      <c r="C244" s="15"/>
-      <c r="D244" s="15"/>
-      <c r="E244" s="15"/>
-      <c r="F244" s="15"/>
-      <c r="G244" s="16"/>
+      <c r="B244" s="16"/>
+      <c r="C244" s="16"/>
+      <c r="D244" s="16"/>
+      <c r="E244" s="16"/>
+      <c r="F244" s="16"/>
+      <c r="G244" s="17"/>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
@@ -6010,26 +6030,26 @@
       <c r="G251" s="2"/>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" s="8" t="s">
+      <c r="A252" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="B252" s="9"/>
-      <c r="C252" s="9"/>
-      <c r="D252" s="9"/>
-      <c r="E252" s="9"/>
-      <c r="F252" s="9"/>
-      <c r="G252" s="10"/>
+      <c r="B252" s="19"/>
+      <c r="C252" s="19"/>
+      <c r="D252" s="19"/>
+      <c r="E252" s="19"/>
+      <c r="F252" s="19"/>
+      <c r="G252" s="20"/>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="14" t="s">
+      <c r="A253" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B253" s="15"/>
-      <c r="C253" s="15"/>
-      <c r="D253" s="15"/>
-      <c r="E253" s="15"/>
-      <c r="F253" s="15"/>
-      <c r="G253" s="16"/>
+      <c r="B253" s="16"/>
+      <c r="C253" s="16"/>
+      <c r="D253" s="16"/>
+      <c r="E253" s="16"/>
+      <c r="F253" s="16"/>
+      <c r="G253" s="17"/>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
@@ -6140,26 +6160,26 @@
       <c r="G259" s="2"/>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A260" s="8" t="s">
+      <c r="A260" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="B260" s="9"/>
-      <c r="C260" s="9"/>
-      <c r="D260" s="9"/>
-      <c r="E260" s="9"/>
-      <c r="F260" s="9"/>
-      <c r="G260" s="10"/>
+      <c r="B260" s="19"/>
+      <c r="C260" s="19"/>
+      <c r="D260" s="19"/>
+      <c r="E260" s="19"/>
+      <c r="F260" s="19"/>
+      <c r="G260" s="20"/>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="14" t="s">
+      <c r="A261" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B261" s="15"/>
-      <c r="C261" s="15"/>
-      <c r="D261" s="15"/>
-      <c r="E261" s="15"/>
-      <c r="F261" s="15"/>
-      <c r="G261" s="16"/>
+      <c r="B261" s="16"/>
+      <c r="C261" s="16"/>
+      <c r="D261" s="16"/>
+      <c r="E261" s="16"/>
+      <c r="F261" s="16"/>
+      <c r="G261" s="17"/>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
@@ -6289,26 +6309,26 @@
       <c r="G268" s="2"/>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="8" t="s">
+      <c r="A269" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="B269" s="9"/>
-      <c r="C269" s="9"/>
-      <c r="D269" s="9"/>
-      <c r="E269" s="9"/>
-      <c r="F269" s="9"/>
-      <c r="G269" s="10"/>
+      <c r="B269" s="19"/>
+      <c r="C269" s="19"/>
+      <c r="D269" s="19"/>
+      <c r="E269" s="19"/>
+      <c r="F269" s="19"/>
+      <c r="G269" s="20"/>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" s="14" t="s">
+      <c r="A270" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B270" s="15"/>
-      <c r="C270" s="15"/>
-      <c r="D270" s="15"/>
-      <c r="E270" s="15"/>
-      <c r="F270" s="15"/>
-      <c r="G270" s="16"/>
+      <c r="B270" s="16"/>
+      <c r="C270" s="16"/>
+      <c r="D270" s="16"/>
+      <c r="E270" s="16"/>
+      <c r="F270" s="16"/>
+      <c r="G270" s="17"/>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
@@ -6421,26 +6441,26 @@
       <c r="G276" s="2"/>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="8" t="s">
+      <c r="A277" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="B277" s="9"/>
-      <c r="C277" s="9"/>
-      <c r="D277" s="9"/>
-      <c r="E277" s="9"/>
-      <c r="F277" s="9"/>
-      <c r="G277" s="10"/>
+      <c r="B277" s="19"/>
+      <c r="C277" s="19"/>
+      <c r="D277" s="19"/>
+      <c r="E277" s="19"/>
+      <c r="F277" s="19"/>
+      <c r="G277" s="20"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="14" t="s">
+      <c r="A278" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B278" s="15"/>
-      <c r="C278" s="15"/>
-      <c r="D278" s="15"/>
-      <c r="E278" s="15"/>
-      <c r="F278" s="15"/>
-      <c r="G278" s="16"/>
+      <c r="B278" s="16"/>
+      <c r="C278" s="16"/>
+      <c r="D278" s="16"/>
+      <c r="E278" s="16"/>
+      <c r="F278" s="16"/>
+      <c r="G278" s="17"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
@@ -6551,26 +6571,26 @@
       <c r="G284" s="2"/>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="8" t="s">
+      <c r="A285" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="B285" s="9"/>
-      <c r="C285" s="9"/>
-      <c r="D285" s="9"/>
-      <c r="E285" s="9"/>
-      <c r="F285" s="9"/>
-      <c r="G285" s="10"/>
+      <c r="B285" s="19"/>
+      <c r="C285" s="19"/>
+      <c r="D285" s="19"/>
+      <c r="E285" s="19"/>
+      <c r="F285" s="19"/>
+      <c r="G285" s="20"/>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="14" t="s">
+      <c r="A286" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B286" s="15"/>
-      <c r="C286" s="15"/>
-      <c r="D286" s="15"/>
-      <c r="E286" s="15"/>
-      <c r="F286" s="15"/>
-      <c r="G286" s="16"/>
+      <c r="B286" s="16"/>
+      <c r="C286" s="16"/>
+      <c r="D286" s="16"/>
+      <c r="E286" s="16"/>
+      <c r="F286" s="16"/>
+      <c r="G286" s="17"/>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
@@ -6890,26 +6910,26 @@
       <c r="G303" s="2"/>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A304" s="8" t="s">
+      <c r="A304" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B304" s="9"/>
-      <c r="C304" s="9"/>
-      <c r="D304" s="9"/>
-      <c r="E304" s="9"/>
-      <c r="F304" s="9"/>
-      <c r="G304" s="10"/>
+      <c r="B304" s="19"/>
+      <c r="C304" s="19"/>
+      <c r="D304" s="19"/>
+      <c r="E304" s="19"/>
+      <c r="F304" s="19"/>
+      <c r="G304" s="20"/>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="14" t="s">
+      <c r="A305" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B305" s="15"/>
-      <c r="C305" s="15"/>
-      <c r="D305" s="15"/>
-      <c r="E305" s="15"/>
-      <c r="F305" s="15"/>
-      <c r="G305" s="16"/>
+      <c r="B305" s="16"/>
+      <c r="C305" s="16"/>
+      <c r="D305" s="16"/>
+      <c r="E305" s="16"/>
+      <c r="F305" s="16"/>
+      <c r="G305" s="17"/>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
@@ -7024,26 +7044,26 @@
       <c r="G311" s="2"/>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A312" s="8" t="s">
+      <c r="A312" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B312" s="9"/>
-      <c r="C312" s="9"/>
-      <c r="D312" s="9"/>
-      <c r="E312" s="9"/>
-      <c r="F312" s="9"/>
-      <c r="G312" s="10"/>
+      <c r="B312" s="19"/>
+      <c r="C312" s="19"/>
+      <c r="D312" s="19"/>
+      <c r="E312" s="19"/>
+      <c r="F312" s="19"/>
+      <c r="G312" s="20"/>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A313" s="14" t="s">
+      <c r="A313" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B313" s="15"/>
-      <c r="C313" s="15"/>
-      <c r="D313" s="15"/>
-      <c r="E313" s="15"/>
-      <c r="F313" s="15"/>
-      <c r="G313" s="16"/>
+      <c r="B313" s="16"/>
+      <c r="C313" s="16"/>
+      <c r="D313" s="16"/>
+      <c r="E313" s="16"/>
+      <c r="F313" s="16"/>
+      <c r="G313" s="17"/>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
@@ -7116,26 +7136,26 @@
       <c r="G317" s="2"/>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A318" s="8" t="s">
+      <c r="A318" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B318" s="9"/>
-      <c r="C318" s="9"/>
-      <c r="D318" s="9"/>
-      <c r="E318" s="9"/>
-      <c r="F318" s="9"/>
-      <c r="G318" s="10"/>
+      <c r="B318" s="19"/>
+      <c r="C318" s="19"/>
+      <c r="D318" s="19"/>
+      <c r="E318" s="19"/>
+      <c r="F318" s="19"/>
+      <c r="G318" s="20"/>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A319" s="14" t="s">
+      <c r="A319" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B319" s="15"/>
-      <c r="C319" s="15"/>
-      <c r="D319" s="15"/>
-      <c r="E319" s="15"/>
-      <c r="F319" s="15"/>
-      <c r="G319" s="16"/>
+      <c r="B319" s="16"/>
+      <c r="C319" s="16"/>
+      <c r="D319" s="16"/>
+      <c r="E319" s="16"/>
+      <c r="F319" s="16"/>
+      <c r="G319" s="17"/>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
@@ -7267,26 +7287,26 @@
       <c r="G326" s="2"/>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A327" s="8" t="s">
+      <c r="A327" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B327" s="9"/>
-      <c r="C327" s="9"/>
-      <c r="D327" s="9"/>
-      <c r="E327" s="9"/>
-      <c r="F327" s="9"/>
-      <c r="G327" s="10"/>
+      <c r="B327" s="19"/>
+      <c r="C327" s="19"/>
+      <c r="D327" s="19"/>
+      <c r="E327" s="19"/>
+      <c r="F327" s="19"/>
+      <c r="G327" s="20"/>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A328" s="14" t="s">
+      <c r="A328" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B328" s="15"/>
-      <c r="C328" s="15"/>
-      <c r="D328" s="15"/>
-      <c r="E328" s="15"/>
-      <c r="F328" s="15"/>
-      <c r="G328" s="16"/>
+      <c r="B328" s="16"/>
+      <c r="C328" s="16"/>
+      <c r="D328" s="16"/>
+      <c r="E328" s="16"/>
+      <c r="F328" s="16"/>
+      <c r="G328" s="17"/>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="4" t="s">
@@ -7359,26 +7379,26 @@
       <c r="G332" s="2"/>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A333" s="8" t="s">
+      <c r="A333" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="B333" s="9"/>
-      <c r="C333" s="9"/>
-      <c r="D333" s="9"/>
-      <c r="E333" s="9"/>
-      <c r="F333" s="9"/>
-      <c r="G333" s="10"/>
+      <c r="B333" s="19"/>
+      <c r="C333" s="19"/>
+      <c r="D333" s="19"/>
+      <c r="E333" s="19"/>
+      <c r="F333" s="19"/>
+      <c r="G333" s="20"/>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A334" s="14" t="s">
+      <c r="A334" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B334" s="15"/>
-      <c r="C334" s="15"/>
-      <c r="D334" s="15"/>
-      <c r="E334" s="15"/>
-      <c r="F334" s="15"/>
-      <c r="G334" s="16"/>
+      <c r="B334" s="16"/>
+      <c r="C334" s="16"/>
+      <c r="D334" s="16"/>
+      <c r="E334" s="16"/>
+      <c r="F334" s="16"/>
+      <c r="G334" s="17"/>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
@@ -7531,26 +7551,26 @@
       <c r="G342" s="2"/>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A343" s="8" t="s">
+      <c r="A343" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B343" s="9"/>
-      <c r="C343" s="9"/>
-      <c r="D343" s="9"/>
-      <c r="E343" s="9"/>
-      <c r="F343" s="9"/>
-      <c r="G343" s="10"/>
+      <c r="B343" s="19"/>
+      <c r="C343" s="19"/>
+      <c r="D343" s="19"/>
+      <c r="E343" s="19"/>
+      <c r="F343" s="19"/>
+      <c r="G343" s="20"/>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A344" s="14" t="s">
+      <c r="A344" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B344" s="15"/>
-      <c r="C344" s="15"/>
-      <c r="D344" s="15"/>
-      <c r="E344" s="15"/>
-      <c r="F344" s="15"/>
-      <c r="G344" s="16"/>
+      <c r="B344" s="16"/>
+      <c r="C344" s="16"/>
+      <c r="D344" s="16"/>
+      <c r="E344" s="16"/>
+      <c r="F344" s="16"/>
+      <c r="G344" s="17"/>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
@@ -7663,26 +7683,26 @@
       <c r="G350" s="2"/>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A351" s="8" t="s">
+      <c r="A351" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="B351" s="9"/>
-      <c r="C351" s="9"/>
-      <c r="D351" s="9"/>
-      <c r="E351" s="9"/>
-      <c r="F351" s="9"/>
-      <c r="G351" s="10"/>
+      <c r="B351" s="19"/>
+      <c r="C351" s="19"/>
+      <c r="D351" s="19"/>
+      <c r="E351" s="19"/>
+      <c r="F351" s="19"/>
+      <c r="G351" s="20"/>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A352" s="14" t="s">
+      <c r="A352" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B352" s="15"/>
-      <c r="C352" s="15"/>
-      <c r="D352" s="15"/>
-      <c r="E352" s="15"/>
-      <c r="F352" s="15"/>
-      <c r="G352" s="16"/>
+      <c r="B352" s="16"/>
+      <c r="C352" s="16"/>
+      <c r="D352" s="16"/>
+      <c r="E352" s="16"/>
+      <c r="F352" s="16"/>
+      <c r="G352" s="17"/>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="4" t="s">
@@ -7833,26 +7853,26 @@
       <c r="G360" s="2"/>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A361" s="8" t="s">
+      <c r="A361" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="B361" s="9"/>
-      <c r="C361" s="9"/>
-      <c r="D361" s="9"/>
-      <c r="E361" s="9"/>
-      <c r="F361" s="9"/>
-      <c r="G361" s="10"/>
+      <c r="B361" s="19"/>
+      <c r="C361" s="19"/>
+      <c r="D361" s="19"/>
+      <c r="E361" s="19"/>
+      <c r="F361" s="19"/>
+      <c r="G361" s="20"/>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362" s="14" t="s">
+      <c r="A362" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B362" s="15"/>
-      <c r="C362" s="15"/>
-      <c r="D362" s="15"/>
-      <c r="E362" s="15"/>
-      <c r="F362" s="15"/>
-      <c r="G362" s="16"/>
+      <c r="B362" s="16"/>
+      <c r="C362" s="16"/>
+      <c r="D362" s="16"/>
+      <c r="E362" s="16"/>
+      <c r="F362" s="16"/>
+      <c r="G362" s="17"/>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" s="4" t="s">
@@ -7965,26 +7985,26 @@
       <c r="G368" s="2"/>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A369" s="11" t="s">
+      <c r="A369" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="B369" s="12"/>
-      <c r="C369" s="12"/>
-      <c r="D369" s="12"/>
-      <c r="E369" s="12"/>
-      <c r="F369" s="12"/>
-      <c r="G369" s="13"/>
+      <c r="B369" s="22"/>
+      <c r="C369" s="22"/>
+      <c r="D369" s="22"/>
+      <c r="E369" s="22"/>
+      <c r="F369" s="22"/>
+      <c r="G369" s="23"/>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A370" s="14" t="s">
+      <c r="A370" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B370" s="15"/>
-      <c r="C370" s="15"/>
-      <c r="D370" s="15"/>
-      <c r="E370" s="15"/>
-      <c r="F370" s="15"/>
-      <c r="G370" s="16"/>
+      <c r="B370" s="16"/>
+      <c r="C370" s="16"/>
+      <c r="D370" s="16"/>
+      <c r="E370" s="16"/>
+      <c r="F370" s="16"/>
+      <c r="G370" s="17"/>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
@@ -8076,26 +8096,26 @@
       <c r="G375" s="2"/>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A376" s="11" t="s">
+      <c r="A376" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="B376" s="12"/>
-      <c r="C376" s="12"/>
-      <c r="D376" s="12"/>
-      <c r="E376" s="12"/>
-      <c r="F376" s="12"/>
-      <c r="G376" s="13"/>
+      <c r="B376" s="22"/>
+      <c r="C376" s="22"/>
+      <c r="D376" s="22"/>
+      <c r="E376" s="22"/>
+      <c r="F376" s="22"/>
+      <c r="G376" s="23"/>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A377" s="14" t="s">
+      <c r="A377" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B377" s="15"/>
-      <c r="C377" s="15"/>
-      <c r="D377" s="15"/>
-      <c r="E377" s="15"/>
-      <c r="F377" s="15"/>
-      <c r="G377" s="16"/>
+      <c r="B377" s="16"/>
+      <c r="C377" s="16"/>
+      <c r="D377" s="16"/>
+      <c r="E377" s="16"/>
+      <c r="F377" s="16"/>
+      <c r="G377" s="17"/>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" s="4" t="s">
@@ -8177,82 +8197,84 @@
       <c r="F381" s="5"/>
       <c r="G381" s="5"/>
     </row>
-    <row r="382" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A382" s="3"/>
-      <c r="B382" s="2"/>
-      <c r="C382" s="2"/>
-      <c r="D382" s="2"/>
-      <c r="E382" s="2"/>
-      <c r="F382" s="2"/>
-      <c r="G382" s="2"/>
-    </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A383" s="8" t="s">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F382" s="5">
+        <v>1</v>
+      </c>
+      <c r="G382" s="5"/>
+    </row>
+    <row r="383" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A383" s="3"/>
+      <c r="B383" s="2"/>
+      <c r="C383" s="2"/>
+      <c r="D383" s="2"/>
+      <c r="E383" s="2"/>
+      <c r="F383" s="2"/>
+      <c r="G383" s="2"/>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B383" s="9"/>
-      <c r="C383" s="9"/>
-      <c r="D383" s="9"/>
-      <c r="E383" s="9"/>
-      <c r="F383" s="9"/>
-      <c r="G383" s="10"/>
-    </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A384" s="14" t="s">
+      <c r="B384" s="19"/>
+      <c r="C384" s="19"/>
+      <c r="D384" s="19"/>
+      <c r="E384" s="19"/>
+      <c r="F384" s="19"/>
+      <c r="G384" s="20"/>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B384" s="15"/>
-      <c r="C384" s="15"/>
-      <c r="D384" s="15"/>
-      <c r="E384" s="15"/>
-      <c r="F384" s="15"/>
-      <c r="G384" s="16"/>
-    </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A385" s="4" t="s">
+      <c r="B385" s="16"/>
+      <c r="C385" s="16"/>
+      <c r="D385" s="16"/>
+      <c r="E385" s="16"/>
+      <c r="F385" s="16"/>
+      <c r="G385" s="17"/>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B385" s="4" t="s">
+      <c r="B386" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C385" s="4" t="s">
+      <c r="C386" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D385" s="4" t="s">
+      <c r="D386" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E385" s="4" t="s">
+      <c r="E386" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F385" s="4" t="s">
+      <c r="F386" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G385" s="4" t="s">
+      <c r="G386" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A386" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B386" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C386" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D386" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E386" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F386" s="5"/>
-      <c r="G386" s="5"/>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
       <c r="B387" s="5" t="s">
         <v>1</v>
@@ -8261,20 +8283,20 @@
         <v>244</v>
       </c>
       <c r="D387" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E387" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F387" s="5"/>
       <c r="G387" s="5"/>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>244</v>
@@ -8283,87 +8305,87 @@
         <v>249</v>
       </c>
       <c r="E388" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F388" s="5"/>
       <c r="G388" s="5"/>
     </row>
-    <row r="389" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A389" s="3"/>
-      <c r="B389" s="2"/>
-      <c r="C389" s="2"/>
-      <c r="D389" s="2"/>
-      <c r="E389" s="2"/>
-      <c r="F389" s="2"/>
-      <c r="G389" s="2"/>
-    </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A390" s="8" t="s">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A389" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C389" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F389" s="5"/>
+      <c r="G389" s="5"/>
+    </row>
+    <row r="390" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A390" s="3"/>
+      <c r="B390" s="2"/>
+      <c r="C390" s="2"/>
+      <c r="D390" s="2"/>
+      <c r="E390" s="2"/>
+      <c r="F390" s="2"/>
+      <c r="G390" s="2"/>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="B390" s="9"/>
-      <c r="C390" s="9"/>
-      <c r="D390" s="9"/>
-      <c r="E390" s="9"/>
-      <c r="F390" s="9"/>
-      <c r="G390" s="10"/>
-    </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A391" s="14" t="s">
+      <c r="B391" s="19"/>
+      <c r="C391" s="19"/>
+      <c r="D391" s="19"/>
+      <c r="E391" s="19"/>
+      <c r="F391" s="19"/>
+      <c r="G391" s="20"/>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B391" s="15"/>
-      <c r="C391" s="15"/>
-      <c r="D391" s="15"/>
-      <c r="E391" s="15"/>
-      <c r="F391" s="15"/>
-      <c r="G391" s="16"/>
-    </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A392" s="4" t="s">
+      <c r="B392" s="16"/>
+      <c r="C392" s="16"/>
+      <c r="D392" s="16"/>
+      <c r="E392" s="16"/>
+      <c r="F392" s="16"/>
+      <c r="G392" s="17"/>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A393" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B392" s="4" t="s">
+      <c r="B393" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C392" s="4" t="s">
+      <c r="C393" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D392" s="4" t="s">
+      <c r="D393" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E392" s="4" t="s">
+      <c r="E393" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F392" s="4" t="s">
+      <c r="F393" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G392" s="4" t="s">
+      <c r="G393" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A393" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B393" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C393" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D393" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E393" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F393" s="5"/>
-      <c r="G393" s="5"/>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
       <c r="B394" s="5" t="s">
         <v>1</v>
@@ -8372,20 +8394,20 @@
         <v>244</v>
       </c>
       <c r="D394" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E394" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F394" s="5"/>
       <c r="G394" s="5"/>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
-        <v>177</v>
+        <v>83</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>178</v>
+        <v>1</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>244</v>
@@ -8394,117 +8416,117 @@
         <v>249</v>
       </c>
       <c r="E395" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F395" s="5"/>
       <c r="G395" s="5"/>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B396" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C396" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D396" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E396" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F396" s="5"/>
+      <c r="G396" s="5"/>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B396" s="5" t="s">
+      <c r="B397" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C396" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D396" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E396" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F396" s="5" t="s">
+      <c r="C397" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D397" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E397" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F397" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G396" s="5"/>
-    </row>
-    <row r="397" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="3"/>
-      <c r="B397" s="2"/>
-      <c r="C397" s="2"/>
-      <c r="D397" s="2"/>
-      <c r="E397" s="2"/>
-      <c r="F397" s="2"/>
-      <c r="G397" s="2"/>
-    </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A398" s="8" t="s">
+      <c r="G397" s="5"/>
+    </row>
+    <row r="398" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A398" s="3"/>
+      <c r="B398" s="2"/>
+      <c r="C398" s="2"/>
+      <c r="D398" s="2"/>
+      <c r="E398" s="2"/>
+      <c r="F398" s="2"/>
+      <c r="G398" s="2"/>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B398" s="9"/>
-      <c r="C398" s="9"/>
-      <c r="D398" s="9"/>
-      <c r="E398" s="9"/>
-      <c r="F398" s="9"/>
-      <c r="G398" s="10"/>
-    </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A399" s="14" t="s">
+      <c r="B399" s="19"/>
+      <c r="C399" s="19"/>
+      <c r="D399" s="19"/>
+      <c r="E399" s="19"/>
+      <c r="F399" s="19"/>
+      <c r="G399" s="20"/>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A400" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B399" s="15"/>
-      <c r="C399" s="15"/>
-      <c r="D399" s="15"/>
-      <c r="E399" s="15"/>
-      <c r="F399" s="15"/>
-      <c r="G399" s="16"/>
-    </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A400" s="4" t="s">
+      <c r="B400" s="16"/>
+      <c r="C400" s="16"/>
+      <c r="D400" s="16"/>
+      <c r="E400" s="16"/>
+      <c r="F400" s="16"/>
+      <c r="G400" s="17"/>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A401" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B400" s="4" t="s">
+      <c r="B401" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C400" s="4" t="s">
+      <c r="C401" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D400" s="4" t="s">
+      <c r="D401" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E400" s="4" t="s">
+      <c r="E401" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F400" s="4" t="s">
+      <c r="F401" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G400" s="4" t="s">
+      <c r="G401" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A401" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B401" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C401" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D401" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E401" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F401" s="5"/>
-      <c r="G401" s="5"/>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="5" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B402" s="5" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D402" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E402" s="5" t="s">
         <v>249</v>
@@ -8512,82 +8534,82 @@
       <c r="F402" s="5"/>
       <c r="G402" s="5"/>
     </row>
-    <row r="403" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A403" s="3"/>
-      <c r="B403" s="2"/>
-      <c r="C403" s="2"/>
-      <c r="D403" s="2"/>
-      <c r="E403" s="2"/>
-      <c r="F403" s="2"/>
-      <c r="G403" s="2"/>
-    </row>
-    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A404" s="8" t="s">
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B403" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C403" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D403" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E403" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F403" s="5"/>
+      <c r="G403" s="5"/>
+    </row>
+    <row r="404" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A404" s="3"/>
+      <c r="B404" s="2"/>
+      <c r="C404" s="2"/>
+      <c r="D404" s="2"/>
+      <c r="E404" s="2"/>
+      <c r="F404" s="2"/>
+      <c r="G404" s="2"/>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="B404" s="9"/>
-      <c r="C404" s="9"/>
-      <c r="D404" s="9"/>
-      <c r="E404" s="9"/>
-      <c r="F404" s="9"/>
-      <c r="G404" s="10"/>
-    </row>
-    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A405" s="14" t="s">
+      <c r="B405" s="19"/>
+      <c r="C405" s="19"/>
+      <c r="D405" s="19"/>
+      <c r="E405" s="19"/>
+      <c r="F405" s="19"/>
+      <c r="G405" s="20"/>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B405" s="15"/>
-      <c r="C405" s="15"/>
-      <c r="D405" s="15"/>
-      <c r="E405" s="15"/>
-      <c r="F405" s="15"/>
-      <c r="G405" s="16"/>
-    </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A406" s="4" t="s">
+      <c r="B406" s="16"/>
+      <c r="C406" s="16"/>
+      <c r="D406" s="16"/>
+      <c r="E406" s="16"/>
+      <c r="F406" s="16"/>
+      <c r="G406" s="17"/>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A407" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B406" s="4" t="s">
+      <c r="B407" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C406" s="4" t="s">
+      <c r="C407" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D406" s="4" t="s">
+      <c r="D407" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E406" s="4" t="s">
+      <c r="E407" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F406" s="4" t="s">
+      <c r="F407" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G406" s="4" t="s">
+      <c r="G407" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A407" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B407" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C407" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D407" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E407" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F407" s="5"/>
-      <c r="G407" s="5"/>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="5" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="B408" s="5" t="s">
         <v>1</v>
@@ -8596,17 +8618,17 @@
         <v>244</v>
       </c>
       <c r="D408" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E408" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F408" s="5"/>
       <c r="G408" s="5"/>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="5" t="s">
-        <v>181</v>
+        <v>65</v>
       </c>
       <c r="B409" s="5" t="s">
         <v>1</v>
@@ -8623,91 +8645,91 @@
       <c r="F409" s="5"/>
       <c r="G409" s="5"/>
     </row>
-    <row r="410" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A410" s="3"/>
-      <c r="B410" s="2"/>
-      <c r="C410" s="2"/>
-      <c r="D410" s="2"/>
-      <c r="E410" s="2"/>
-      <c r="F410" s="2"/>
-      <c r="G410" s="2"/>
-    </row>
-    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A411" s="8" t="s">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A410" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B410" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C410" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D410" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F410" s="5"/>
+      <c r="G410" s="5"/>
+    </row>
+    <row r="411" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A411" s="3"/>
+      <c r="B411" s="2"/>
+      <c r="C411" s="2"/>
+      <c r="D411" s="2"/>
+      <c r="E411" s="2"/>
+      <c r="F411" s="2"/>
+      <c r="G411" s="2"/>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A412" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="B411" s="9"/>
-      <c r="C411" s="9"/>
-      <c r="D411" s="9"/>
-      <c r="E411" s="9"/>
-      <c r="F411" s="9"/>
-      <c r="G411" s="10"/>
-    </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A412" s="14" t="s">
+      <c r="B412" s="19"/>
+      <c r="C412" s="19"/>
+      <c r="D412" s="19"/>
+      <c r="E412" s="19"/>
+      <c r="F412" s="19"/>
+      <c r="G412" s="20"/>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A413" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B412" s="15"/>
-      <c r="C412" s="15"/>
-      <c r="D412" s="15"/>
-      <c r="E412" s="15"/>
-      <c r="F412" s="15"/>
-      <c r="G412" s="16"/>
-    </row>
-    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A413" s="4" t="s">
+      <c r="B413" s="16"/>
+      <c r="C413" s="16"/>
+      <c r="D413" s="16"/>
+      <c r="E413" s="16"/>
+      <c r="F413" s="16"/>
+      <c r="G413" s="17"/>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A414" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B413" s="4" t="s">
+      <c r="B414" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C413" s="4" t="s">
+      <c r="C414" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D413" s="4" t="s">
+      <c r="D414" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E413" s="4" t="s">
+      <c r="E414" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F413" s="4" t="s">
+      <c r="F414" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G413" s="4" t="s">
+      <c r="G414" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A414" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B414" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C414" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D414" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E414" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F414" s="5"/>
-      <c r="G414" s="5"/>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D415" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E415" s="5" t="s">
         <v>249</v>
@@ -8715,82 +8737,82 @@
       <c r="F415" s="5"/>
       <c r="G415" s="5"/>
     </row>
-    <row r="416" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A416" s="3"/>
-      <c r="B416" s="2"/>
-      <c r="C416" s="2"/>
-      <c r="D416" s="2"/>
-      <c r="E416" s="2"/>
-      <c r="F416" s="2"/>
-      <c r="G416" s="2"/>
-    </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A417" s="8" t="s">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A416" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B416" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C416" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D416" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F416" s="5"/>
+      <c r="G416" s="5"/>
+    </row>
+    <row r="417" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A417" s="3"/>
+      <c r="B417" s="2"/>
+      <c r="C417" s="2"/>
+      <c r="D417" s="2"/>
+      <c r="E417" s="2"/>
+      <c r="F417" s="2"/>
+      <c r="G417" s="2"/>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A418" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="B417" s="9"/>
-      <c r="C417" s="9"/>
-      <c r="D417" s="9"/>
-      <c r="E417" s="9"/>
-      <c r="F417" s="9"/>
-      <c r="G417" s="10"/>
-    </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A418" s="14" t="s">
+      <c r="B418" s="19"/>
+      <c r="C418" s="19"/>
+      <c r="D418" s="19"/>
+      <c r="E418" s="19"/>
+      <c r="F418" s="19"/>
+      <c r="G418" s="20"/>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A419" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B418" s="15"/>
-      <c r="C418" s="15"/>
-      <c r="D418" s="15"/>
-      <c r="E418" s="15"/>
-      <c r="F418" s="15"/>
-      <c r="G418" s="16"/>
-    </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A419" s="4" t="s">
+      <c r="B419" s="16"/>
+      <c r="C419" s="16"/>
+      <c r="D419" s="16"/>
+      <c r="E419" s="16"/>
+      <c r="F419" s="16"/>
+      <c r="G419" s="17"/>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A420" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B419" s="4" t="s">
+      <c r="B420" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C419" s="4" t="s">
+      <c r="C420" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D419" s="4" t="s">
+      <c r="D420" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E419" s="4" t="s">
+      <c r="E420" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F419" s="4" t="s">
+      <c r="F420" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G419" s="4" t="s">
+      <c r="G420" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A420" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B420" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C420" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D420" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E420" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F420" s="5"/>
-      <c r="G420" s="5"/>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="B421" s="5" t="s">
         <v>1</v>
@@ -8799,20 +8821,20 @@
         <v>244</v>
       </c>
       <c r="D421" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E421" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F421" s="5"/>
       <c r="G421" s="5"/>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>184</v>
+        <v>1</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>244</v>
@@ -8821,108 +8843,108 @@
         <v>249</v>
       </c>
       <c r="E422" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F422" s="5"/>
       <c r="G422" s="5"/>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B423" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C423" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D423" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F423" s="5"/>
+      <c r="G423" s="5"/>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A424" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B423" s="5" t="s">
+      <c r="B424" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C423" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D423" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E423" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F423" s="5">
+      <c r="C424" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F424" s="5">
         <v>0</v>
       </c>
-      <c r="G423" s="5"/>
-    </row>
-    <row r="424" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A424" s="3"/>
-      <c r="B424" s="2"/>
-      <c r="C424" s="2"/>
-      <c r="D424" s="2"/>
-      <c r="E424" s="2"/>
-      <c r="F424" s="2"/>
-      <c r="G424" s="2"/>
-    </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A425" s="8" t="s">
+      <c r="G424" s="5"/>
+    </row>
+    <row r="425" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A425" s="3"/>
+      <c r="B425" s="2"/>
+      <c r="C425" s="2"/>
+      <c r="D425" s="2"/>
+      <c r="E425" s="2"/>
+      <c r="F425" s="2"/>
+      <c r="G425" s="2"/>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A426" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="B425" s="9"/>
-      <c r="C425" s="9"/>
-      <c r="D425" s="9"/>
-      <c r="E425" s="9"/>
-      <c r="F425" s="9"/>
-      <c r="G425" s="10"/>
-    </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A426" s="14" t="s">
+      <c r="B426" s="19"/>
+      <c r="C426" s="19"/>
+      <c r="D426" s="19"/>
+      <c r="E426" s="19"/>
+      <c r="F426" s="19"/>
+      <c r="G426" s="20"/>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A427" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B426" s="15"/>
-      <c r="C426" s="15"/>
-      <c r="D426" s="15"/>
-      <c r="E426" s="15"/>
-      <c r="F426" s="15"/>
-      <c r="G426" s="16"/>
-    </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A427" s="4" t="s">
+      <c r="B427" s="16"/>
+      <c r="C427" s="16"/>
+      <c r="D427" s="16"/>
+      <c r="E427" s="16"/>
+      <c r="F427" s="16"/>
+      <c r="G427" s="17"/>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A428" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B427" s="4" t="s">
+      <c r="B428" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C427" s="4" t="s">
+      <c r="C428" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D427" s="4" t="s">
+      <c r="D428" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E427" s="4" t="s">
+      <c r="E428" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F427" s="4" t="s">
+      <c r="F428" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G427" s="4" t="s">
+      <c r="G428" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A428" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B428" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C428" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D428" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E428" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F428" s="5"/>
-      <c r="G428" s="5"/>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" s="5" t="s">
-        <v>84</v>
+        <v>185</v>
       </c>
       <c r="B429" s="5" t="s">
         <v>1</v>
@@ -8931,20 +8953,20 @@
         <v>244</v>
       </c>
       <c r="D429" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E429" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F429" s="5"/>
       <c r="G429" s="5"/>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" s="5" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B430" s="5" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>244</v>
@@ -8953,117 +8975,117 @@
         <v>249</v>
       </c>
       <c r="E430" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F430" s="5"/>
       <c r="G430" s="5"/>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B431" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C431" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D431" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E431" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F431" s="5"/>
+      <c r="G431" s="5"/>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A432" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B431" s="5" t="s">
+      <c r="B432" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C431" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D431" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E431" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F431" s="5">
+      <c r="C432" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D432" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F432" s="5">
         <v>0</v>
       </c>
-      <c r="G431" s="5"/>
-    </row>
-    <row r="432" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A432" s="3"/>
-      <c r="B432" s="2"/>
-      <c r="C432" s="2"/>
-      <c r="D432" s="2"/>
-      <c r="E432" s="2"/>
-      <c r="F432" s="2"/>
-      <c r="G432" s="2"/>
-    </row>
-    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A433" s="8" t="s">
+      <c r="G432" s="5"/>
+    </row>
+    <row r="433" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A433" s="3"/>
+      <c r="B433" s="2"/>
+      <c r="C433" s="2"/>
+      <c r="D433" s="2"/>
+      <c r="E433" s="2"/>
+      <c r="F433" s="2"/>
+      <c r="G433" s="2"/>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A434" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B433" s="9"/>
-      <c r="C433" s="9"/>
-      <c r="D433" s="9"/>
-      <c r="E433" s="9"/>
-      <c r="F433" s="9"/>
-      <c r="G433" s="10"/>
-    </row>
-    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A434" s="14" t="s">
+      <c r="B434" s="19"/>
+      <c r="C434" s="19"/>
+      <c r="D434" s="19"/>
+      <c r="E434" s="19"/>
+      <c r="F434" s="19"/>
+      <c r="G434" s="20"/>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A435" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B434" s="15"/>
-      <c r="C434" s="15"/>
-      <c r="D434" s="15"/>
-      <c r="E434" s="15"/>
-      <c r="F434" s="15"/>
-      <c r="G434" s="16"/>
-    </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A435" s="4" t="s">
+      <c r="B435" s="16"/>
+      <c r="C435" s="16"/>
+      <c r="D435" s="16"/>
+      <c r="E435" s="16"/>
+      <c r="F435" s="16"/>
+      <c r="G435" s="17"/>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A436" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B435" s="4" t="s">
+      <c r="B436" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C435" s="4" t="s">
+      <c r="C436" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D435" s="4" t="s">
+      <c r="D436" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E435" s="4" t="s">
+      <c r="E436" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F435" s="4" t="s">
+      <c r="F436" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G435" s="4" t="s">
+      <c r="G436" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A436" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B436" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C436" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D436" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E436" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="F436" s="5"/>
-      <c r="G436" s="5"/>
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D437" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E437" s="5" t="s">
         <v>249</v>
@@ -9071,236 +9093,381 @@
       <c r="F437" s="5"/>
       <c r="G437" s="5"/>
     </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A439" s="17" t="s">
+    <row r="438" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A438" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B438" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C438" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D438" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E438" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F438" s="5"/>
+      <c r="G438" s="5"/>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A440" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B439" s="19"/>
-      <c r="C439" s="19"/>
-      <c r="D439" s="19"/>
-      <c r="E439" s="19"/>
-      <c r="F439" s="19"/>
-      <c r="G439" s="19"/>
-    </row>
-    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A440" s="17" t="s">
+      <c r="B440" s="13"/>
+      <c r="C440" s="13"/>
+      <c r="D440" s="13"/>
+      <c r="E440" s="13"/>
+      <c r="F440" s="13"/>
+      <c r="G440" s="13"/>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A441" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B440" s="17"/>
-      <c r="C440" s="17"/>
-      <c r="D440" s="17"/>
-      <c r="E440" s="17"/>
-      <c r="F440" s="17"/>
-      <c r="G440" s="17"/>
-    </row>
-    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A441" s="20" t="s">
+      <c r="B441" s="12"/>
+      <c r="C441" s="12"/>
+      <c r="D441" s="12"/>
+      <c r="E441" s="12"/>
+      <c r="F441" s="12"/>
+      <c r="G441" s="12"/>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A442" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B441" s="20" t="s">
+      <c r="B442" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C441" s="20" t="s">
+      <c r="C442" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D441" s="20" t="s">
+      <c r="D442" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="E441" s="20" t="s">
+      <c r="E442" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F441" s="20" t="s">
+      <c r="F442" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="G441" s="20" t="s">
+      <c r="G442" s="8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A442" s="21" t="s">
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A443" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B442" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C442" s="21" t="s">
+      <c r="B443" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C443" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D442" s="21" t="s">
+      <c r="D443" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E442" s="21" t="s">
+      <c r="E443" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F443" s="10"/>
+      <c r="G443" s="10"/>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A444" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B444" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C444" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D444" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E444" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F444" s="10"/>
+      <c r="G444" s="10"/>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A445" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B445" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C445" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D445" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E445" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F445" s="10"/>
+      <c r="G445" s="10"/>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A446" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F442" s="22"/>
-      <c r="G442" s="22"/>
-    </row>
-    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A443" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B443" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C443" s="21" t="s">
+      <c r="B446" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C446" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D443" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E443" s="21" t="s">
+      <c r="D446" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E446" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F446" s="10"/>
+      <c r="G446" s="10"/>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A447" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B447" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C447" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="F443" s="22"/>
-      <c r="G443" s="22"/>
-    </row>
-    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A444" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B444" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C444" s="21" t="s">
+      <c r="D447" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E447" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F447" s="10"/>
+      <c r="G447" s="10"/>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A448" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B448" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C448" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D444" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E444" s="21" t="s">
+      <c r="D448" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E448" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F448" s="10"/>
+      <c r="G448" s="10"/>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A449" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B449" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C449" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D449" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E449" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F449" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G449" s="10"/>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A451" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B451" s="13"/>
+      <c r="C451" s="13"/>
+      <c r="D451" s="13"/>
+      <c r="E451" s="13"/>
+      <c r="F451" s="13"/>
+      <c r="G451" s="13"/>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A452" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B452" s="12"/>
+      <c r="C452" s="12"/>
+      <c r="D452" s="12"/>
+      <c r="E452" s="12"/>
+      <c r="F452" s="12"/>
+      <c r="G452" s="12"/>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A453" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B453" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C453" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D453" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E453" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="F453" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="G453" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A454" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B454" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C454" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="F444" s="22"/>
-      <c r="G444" s="22"/>
-    </row>
-    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A445" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="B445" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="C445" s="21" t="s">
+      <c r="D454" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D445" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E445" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="F445" s="22"/>
-      <c r="G445" s="22"/>
-    </row>
-    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A446" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="B446" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="C446" s="23" t="s">
+      <c r="E454" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F454" s="10"/>
+      <c r="G454" s="10"/>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A455" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B455" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C455" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D446" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E446" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="F446" s="22"/>
-      <c r="G446" s="22"/>
-    </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A447" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="B447" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="C447" s="21" t="s">
+      <c r="D455" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E455" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F455" s="10"/>
+      <c r="G455" s="10"/>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A456" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B456" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C456" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D447" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E447" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="F447" s="22"/>
-      <c r="G447" s="22"/>
-    </row>
-    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A448" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="B448" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C448" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="D448" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="E448" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="F448" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G448" s="22"/>
+      <c r="D456" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E456" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F456" s="10"/>
+      <c r="G456" s="10"/>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A457" s="24"/>
+      <c r="B457" s="24"/>
+      <c r="C457" s="24"/>
+      <c r="D457" s="24"/>
+      <c r="E457" s="24"/>
+      <c r="F457" s="25"/>
+      <c r="G457" s="25"/>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A458" s="24"/>
+      <c r="B458" s="24"/>
+      <c r="C458" s="26"/>
+      <c r="D458" s="24"/>
+      <c r="E458" s="24"/>
+      <c r="F458" s="25"/>
+      <c r="G458" s="25"/>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A459" s="24"/>
+      <c r="B459" s="24"/>
+      <c r="C459" s="24"/>
+      <c r="D459" s="24"/>
+      <c r="E459" s="24"/>
+      <c r="F459" s="25"/>
+      <c r="G459" s="25"/>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A460" s="24"/>
+      <c r="B460" s="24"/>
+      <c r="C460" s="24"/>
+      <c r="D460" s="24"/>
+      <c r="E460" s="24"/>
+      <c r="F460" s="6"/>
+      <c r="G460" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="106">
-    <mergeCell ref="A439:G439"/>
-    <mergeCell ref="A440:G440"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A137:G137"/>
-    <mergeCell ref="A146:G146"/>
-    <mergeCell ref="A152:G152"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="A114:G114"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A89:G89"/>
-    <mergeCell ref="A136:G136"/>
-    <mergeCell ref="A129:G129"/>
-    <mergeCell ref="A123:G123"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="A124:G124"/>
-    <mergeCell ref="A130:G130"/>
+  <mergeCells count="108">
+    <mergeCell ref="A451:G451"/>
+    <mergeCell ref="A452:G452"/>
+    <mergeCell ref="A412:G412"/>
     <mergeCell ref="A434:G434"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A370:G370"/>
-    <mergeCell ref="A377:G377"/>
+    <mergeCell ref="A418:G418"/>
+    <mergeCell ref="A426:G426"/>
+    <mergeCell ref="A369:G369"/>
+    <mergeCell ref="A376:G376"/>
     <mergeCell ref="A384:G384"/>
     <mergeCell ref="A391:G391"/>
     <mergeCell ref="A399:G399"/>
-    <mergeCell ref="A405:G405"/>
-    <mergeCell ref="A404:G404"/>
-    <mergeCell ref="A319:G319"/>
-    <mergeCell ref="A328:G328"/>
-    <mergeCell ref="A334:G334"/>
-    <mergeCell ref="A344:G344"/>
-    <mergeCell ref="A352:G352"/>
-    <mergeCell ref="A362:G362"/>
-    <mergeCell ref="A343:G343"/>
-    <mergeCell ref="A361:G361"/>
+    <mergeCell ref="A413:G413"/>
+    <mergeCell ref="A419:G419"/>
+    <mergeCell ref="A427:G427"/>
+    <mergeCell ref="A187:G187"/>
+    <mergeCell ref="A193:G193"/>
+    <mergeCell ref="A199:G199"/>
+    <mergeCell ref="A260:G260"/>
+    <mergeCell ref="A269:G269"/>
+    <mergeCell ref="A277:G277"/>
+    <mergeCell ref="A304:G304"/>
+    <mergeCell ref="A333:G333"/>
+    <mergeCell ref="A327:G327"/>
+    <mergeCell ref="A312:G312"/>
+    <mergeCell ref="A318:G318"/>
+    <mergeCell ref="A205:G205"/>
+    <mergeCell ref="A261:G261"/>
+    <mergeCell ref="A270:G270"/>
+    <mergeCell ref="A278:G278"/>
+    <mergeCell ref="A286:G286"/>
+    <mergeCell ref="A305:G305"/>
+    <mergeCell ref="A313:G313"/>
+    <mergeCell ref="A285:G285"/>
+    <mergeCell ref="A244:G244"/>
+    <mergeCell ref="A253:G253"/>
+    <mergeCell ref="A252:G252"/>
     <mergeCell ref="A351:G351"/>
     <mergeCell ref="A107:G107"/>
     <mergeCell ref="A113:G113"/>
@@ -9325,40 +9492,54 @@
     <mergeCell ref="A167:G167"/>
     <mergeCell ref="A173:G173"/>
     <mergeCell ref="A180:G180"/>
-    <mergeCell ref="A187:G187"/>
-    <mergeCell ref="A193:G193"/>
-    <mergeCell ref="A199:G199"/>
-    <mergeCell ref="A260:G260"/>
-    <mergeCell ref="A269:G269"/>
-    <mergeCell ref="A277:G277"/>
-    <mergeCell ref="A304:G304"/>
-    <mergeCell ref="A333:G333"/>
-    <mergeCell ref="A327:G327"/>
-    <mergeCell ref="A312:G312"/>
-    <mergeCell ref="A318:G318"/>
-    <mergeCell ref="A205:G205"/>
-    <mergeCell ref="A261:G261"/>
-    <mergeCell ref="A270:G270"/>
-    <mergeCell ref="A278:G278"/>
-    <mergeCell ref="A286:G286"/>
-    <mergeCell ref="A305:G305"/>
-    <mergeCell ref="A313:G313"/>
-    <mergeCell ref="A285:G285"/>
-    <mergeCell ref="A244:G244"/>
-    <mergeCell ref="A253:G253"/>
-    <mergeCell ref="A252:G252"/>
-    <mergeCell ref="A411:G411"/>
-    <mergeCell ref="A433:G433"/>
-    <mergeCell ref="A417:G417"/>
-    <mergeCell ref="A425:G425"/>
-    <mergeCell ref="A369:G369"/>
-    <mergeCell ref="A376:G376"/>
-    <mergeCell ref="A383:G383"/>
-    <mergeCell ref="A390:G390"/>
-    <mergeCell ref="A398:G398"/>
-    <mergeCell ref="A412:G412"/>
-    <mergeCell ref="A418:G418"/>
-    <mergeCell ref="A426:G426"/>
+    <mergeCell ref="A136:G136"/>
+    <mergeCell ref="A129:G129"/>
+    <mergeCell ref="A123:G123"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="A130:G130"/>
+    <mergeCell ref="A435:G435"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A370:G370"/>
+    <mergeCell ref="A377:G377"/>
+    <mergeCell ref="A385:G385"/>
+    <mergeCell ref="A392:G392"/>
+    <mergeCell ref="A400:G400"/>
+    <mergeCell ref="A406:G406"/>
+    <mergeCell ref="A405:G405"/>
+    <mergeCell ref="A319:G319"/>
+    <mergeCell ref="A328:G328"/>
+    <mergeCell ref="A334:G334"/>
+    <mergeCell ref="A344:G344"/>
+    <mergeCell ref="A352:G352"/>
+    <mergeCell ref="A362:G362"/>
+    <mergeCell ref="A343:G343"/>
+    <mergeCell ref="A361:G361"/>
+    <mergeCell ref="A440:G440"/>
+    <mergeCell ref="A441:G441"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A137:G137"/>
+    <mergeCell ref="A146:G146"/>
+    <mergeCell ref="A152:G152"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A108:G108"/>
+    <mergeCell ref="A114:G114"/>
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A89:G89"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adiciona a tabela tbl_topico_sobre_empresa
</commit_message>
<xml_diff>
--- a/database/dicionario/dicionario_de_dados.xltx.xlsx
+++ b/database/dicionario/dicionario_de_dados.xltx.xlsx
@@ -816,13 +816,13 @@
     <t>VARCHAR(2400)</t>
   </si>
   <si>
-    <t>Tabela: tbl_topico_empresa-</t>
-  </si>
-  <si>
-    <t>id_topico_empresa</t>
-  </si>
-  <si>
-    <t>topico_empresa</t>
+    <t>Tabela: tbl_topico_sobre_empresa-</t>
+  </si>
+  <si>
+    <t>id_topico_sobre_empresa</t>
+  </si>
+  <si>
+    <t>topico_sobre_empresa</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1477,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1489,28 +1510,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1870,7 +1870,7 @@
   <dimension ref="A1:G467"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A444" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J462" sqref="J462"/>
+      <selection activeCell="A466" sqref="A466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,26 +1885,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2148,26 +2148,26 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2259,26 +2259,26 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -2469,26 +2469,26 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -2713,26 +2713,26 @@
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="17"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="24"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -2805,26 +2805,26 @@
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="21"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="18"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="17"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="24"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
@@ -2897,26 +2897,26 @@
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="21"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="17"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="24"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
@@ -3103,26 +3103,26 @@
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="21"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="17"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="24"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
@@ -3195,26 +3195,26 @@
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="21"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="17"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="24"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
@@ -3367,26 +3367,26 @@
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
+      <c r="A89" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="21"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="18"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B90" s="16"/>
-      <c r="C90" s="16"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="17"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="24"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
@@ -3691,26 +3691,26 @@
       <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="19" t="s">
+      <c r="A107" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="B107" s="20"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="21"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="18"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="15" t="s">
+      <c r="A108" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="16"/>
-      <c r="C108" s="16"/>
-      <c r="D108" s="16"/>
-      <c r="E108" s="16"/>
-      <c r="F108" s="16"/>
-      <c r="G108" s="17"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="23"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="24"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
@@ -3783,26 +3783,26 @@
       <c r="G112" s="2"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B113" s="20"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="21"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="18"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="15" t="s">
+      <c r="A114" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B114" s="16"/>
-      <c r="C114" s="16"/>
-      <c r="D114" s="16"/>
-      <c r="E114" s="16"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="17"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="24"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
@@ -3953,26 +3953,26 @@
       <c r="G122" s="2"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="19" t="s">
+      <c r="A123" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B123" s="20"/>
-      <c r="C123" s="20"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="21"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="17"/>
+      <c r="G123" s="18"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="15" t="s">
+      <c r="A124" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B124" s="16"/>
-      <c r="C124" s="16"/>
-      <c r="D124" s="16"/>
-      <c r="E124" s="16"/>
-      <c r="F124" s="16"/>
-      <c r="G124" s="17"/>
+      <c r="B124" s="23"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="24"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
@@ -4045,26 +4045,26 @@
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="19" t="s">
+      <c r="A129" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B129" s="20"/>
-      <c r="C129" s="20"/>
-      <c r="D129" s="20"/>
-      <c r="E129" s="20"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="21"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="17"/>
+      <c r="G129" s="18"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="15" t="s">
+      <c r="A130" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B130" s="16"/>
-      <c r="C130" s="16"/>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="16"/>
-      <c r="G130" s="17"/>
+      <c r="B130" s="23"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="24"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
@@ -4175,26 +4175,26 @@
       <c r="G136" s="2"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="19" t="s">
+      <c r="A137" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B137" s="20"/>
-      <c r="C137" s="20"/>
-      <c r="D137" s="20"/>
-      <c r="E137" s="20"/>
-      <c r="F137" s="20"/>
-      <c r="G137" s="21"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="18"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
+      <c r="A138" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B138" s="16"/>
-      <c r="C138" s="16"/>
-      <c r="D138" s="16"/>
-      <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
-      <c r="G138" s="17"/>
+      <c r="B138" s="23"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="24"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
@@ -4326,26 +4326,26 @@
       <c r="G145" s="2"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="19" t="s">
+      <c r="A146" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="B146" s="20"/>
-      <c r="C146" s="20"/>
-      <c r="D146" s="20"/>
-      <c r="E146" s="20"/>
-      <c r="F146" s="20"/>
-      <c r="G146" s="21"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="17"/>
+      <c r="G146" s="18"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="15" t="s">
+      <c r="A147" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="16"/>
-      <c r="C147" s="16"/>
-      <c r="D147" s="16"/>
-      <c r="E147" s="16"/>
-      <c r="F147" s="16"/>
-      <c r="G147" s="17"/>
+      <c r="B147" s="23"/>
+      <c r="C147" s="23"/>
+      <c r="D147" s="23"/>
+      <c r="E147" s="23"/>
+      <c r="F147" s="23"/>
+      <c r="G147" s="24"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
@@ -4418,26 +4418,26 @@
       <c r="G151" s="2"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="19" t="s">
+      <c r="A152" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B152" s="20"/>
-      <c r="C152" s="20"/>
-      <c r="D152" s="20"/>
-      <c r="E152" s="20"/>
-      <c r="F152" s="20"/>
-      <c r="G152" s="21"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="17"/>
+      <c r="G152" s="18"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="15" t="s">
+      <c r="A153" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B153" s="16"/>
-      <c r="C153" s="16"/>
-      <c r="D153" s="16"/>
-      <c r="E153" s="16"/>
-      <c r="F153" s="16"/>
-      <c r="G153" s="17"/>
+      <c r="B153" s="23"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="23"/>
+      <c r="E153" s="23"/>
+      <c r="F153" s="23"/>
+      <c r="G153" s="24"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
@@ -4550,26 +4550,26 @@
       <c r="G159" s="2"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="19" t="s">
+      <c r="A160" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B160" s="20"/>
-      <c r="C160" s="20"/>
-      <c r="D160" s="20"/>
-      <c r="E160" s="20"/>
-      <c r="F160" s="20"/>
-      <c r="G160" s="21"/>
+      <c r="B160" s="17"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17"/>
+      <c r="G160" s="18"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="15" t="s">
+      <c r="A161" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B161" s="16"/>
-      <c r="C161" s="16"/>
-      <c r="D161" s="16"/>
-      <c r="E161" s="16"/>
-      <c r="F161" s="16"/>
-      <c r="G161" s="17"/>
+      <c r="B161" s="23"/>
+      <c r="C161" s="23"/>
+      <c r="D161" s="23"/>
+      <c r="E161" s="23"/>
+      <c r="F161" s="23"/>
+      <c r="G161" s="24"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
@@ -4661,26 +4661,26 @@
       <c r="G166" s="2"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="19" t="s">
+      <c r="A167" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="B167" s="20"/>
-      <c r="C167" s="20"/>
-      <c r="D167" s="20"/>
-      <c r="E167" s="20"/>
-      <c r="F167" s="20"/>
-      <c r="G167" s="21"/>
+      <c r="B167" s="17"/>
+      <c r="C167" s="17"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="17"/>
+      <c r="G167" s="18"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" s="15" t="s">
+      <c r="A168" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B168" s="16"/>
-      <c r="C168" s="16"/>
-      <c r="D168" s="16"/>
-      <c r="E168" s="16"/>
-      <c r="F168" s="16"/>
-      <c r="G168" s="17"/>
+      <c r="B168" s="23"/>
+      <c r="C168" s="23"/>
+      <c r="D168" s="23"/>
+      <c r="E168" s="23"/>
+      <c r="F168" s="23"/>
+      <c r="G168" s="24"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
@@ -4753,26 +4753,26 @@
       <c r="G172" s="2"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="19" t="s">
+      <c r="A173" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="B173" s="20"/>
-      <c r="C173" s="20"/>
-      <c r="D173" s="20"/>
-      <c r="E173" s="20"/>
-      <c r="F173" s="20"/>
-      <c r="G173" s="21"/>
+      <c r="B173" s="17"/>
+      <c r="C173" s="17"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="18"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="15" t="s">
+      <c r="A174" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B174" s="16"/>
-      <c r="C174" s="16"/>
-      <c r="D174" s="16"/>
-      <c r="E174" s="16"/>
-      <c r="F174" s="16"/>
-      <c r="G174" s="17"/>
+      <c r="B174" s="23"/>
+      <c r="C174" s="23"/>
+      <c r="D174" s="23"/>
+      <c r="E174" s="23"/>
+      <c r="F174" s="23"/>
+      <c r="G174" s="24"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
@@ -4864,26 +4864,26 @@
       <c r="G179" s="2"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="19" t="s">
+      <c r="A180" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B180" s="20"/>
-      <c r="C180" s="20"/>
-      <c r="D180" s="20"/>
-      <c r="E180" s="20"/>
-      <c r="F180" s="20"/>
-      <c r="G180" s="21"/>
+      <c r="B180" s="17"/>
+      <c r="C180" s="17"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="17"/>
+      <c r="G180" s="18"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="15" t="s">
+      <c r="A181" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B181" s="16"/>
-      <c r="C181" s="16"/>
-      <c r="D181" s="16"/>
-      <c r="E181" s="16"/>
-      <c r="F181" s="16"/>
-      <c r="G181" s="17"/>
+      <c r="B181" s="23"/>
+      <c r="C181" s="23"/>
+      <c r="D181" s="23"/>
+      <c r="E181" s="23"/>
+      <c r="F181" s="23"/>
+      <c r="G181" s="24"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
@@ -4975,26 +4975,26 @@
       <c r="G186" s="2"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="19" t="s">
+      <c r="A187" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="B187" s="20"/>
-      <c r="C187" s="20"/>
-      <c r="D187" s="20"/>
-      <c r="E187" s="20"/>
-      <c r="F187" s="20"/>
-      <c r="G187" s="21"/>
+      <c r="B187" s="17"/>
+      <c r="C187" s="17"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="17"/>
+      <c r="G187" s="18"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="15" t="s">
+      <c r="A188" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B188" s="16"/>
-      <c r="C188" s="16"/>
-      <c r="D188" s="16"/>
-      <c r="E188" s="16"/>
-      <c r="F188" s="16"/>
-      <c r="G188" s="17"/>
+      <c r="B188" s="23"/>
+      <c r="C188" s="23"/>
+      <c r="D188" s="23"/>
+      <c r="E188" s="23"/>
+      <c r="F188" s="23"/>
+      <c r="G188" s="24"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
@@ -5067,26 +5067,26 @@
       <c r="G192" s="2"/>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" s="19" t="s">
+      <c r="A193" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B193" s="20"/>
-      <c r="C193" s="20"/>
-      <c r="D193" s="20"/>
-      <c r="E193" s="20"/>
-      <c r="F193" s="20"/>
-      <c r="G193" s="21"/>
+      <c r="B193" s="17"/>
+      <c r="C193" s="17"/>
+      <c r="D193" s="17"/>
+      <c r="E193" s="17"/>
+      <c r="F193" s="17"/>
+      <c r="G193" s="18"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A194" s="15" t="s">
+      <c r="A194" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B194" s="16"/>
-      <c r="C194" s="16"/>
-      <c r="D194" s="16"/>
-      <c r="E194" s="16"/>
-      <c r="F194" s="16"/>
-      <c r="G194" s="17"/>
+      <c r="B194" s="23"/>
+      <c r="C194" s="23"/>
+      <c r="D194" s="23"/>
+      <c r="E194" s="23"/>
+      <c r="F194" s="23"/>
+      <c r="G194" s="24"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
@@ -5159,26 +5159,26 @@
       <c r="G198" s="2"/>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="19" t="s">
+      <c r="A199" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B199" s="20"/>
-      <c r="C199" s="20"/>
-      <c r="D199" s="20"/>
-      <c r="E199" s="20"/>
-      <c r="F199" s="20"/>
-      <c r="G199" s="21"/>
+      <c r="B199" s="17"/>
+      <c r="C199" s="17"/>
+      <c r="D199" s="17"/>
+      <c r="E199" s="17"/>
+      <c r="F199" s="17"/>
+      <c r="G199" s="18"/>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A200" s="15" t="s">
+      <c r="A200" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B200" s="16"/>
-      <c r="C200" s="16"/>
-      <c r="D200" s="16"/>
-      <c r="E200" s="16"/>
-      <c r="F200" s="16"/>
-      <c r="G200" s="17"/>
+      <c r="B200" s="23"/>
+      <c r="C200" s="23"/>
+      <c r="D200" s="23"/>
+      <c r="E200" s="23"/>
+      <c r="F200" s="23"/>
+      <c r="G200" s="24"/>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
@@ -5270,26 +5270,26 @@
       <c r="G205" s="2"/>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A206" s="19" t="s">
+      <c r="A206" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B206" s="20"/>
-      <c r="C206" s="20"/>
-      <c r="D206" s="20"/>
-      <c r="E206" s="20"/>
-      <c r="F206" s="20"/>
-      <c r="G206" s="21"/>
+      <c r="B206" s="17"/>
+      <c r="C206" s="17"/>
+      <c r="D206" s="17"/>
+      <c r="E206" s="17"/>
+      <c r="F206" s="17"/>
+      <c r="G206" s="18"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A207" s="15" t="s">
+      <c r="A207" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B207" s="16"/>
-      <c r="C207" s="16"/>
-      <c r="D207" s="16"/>
-      <c r="E207" s="16"/>
-      <c r="F207" s="16"/>
-      <c r="G207" s="17"/>
+      <c r="B207" s="23"/>
+      <c r="C207" s="23"/>
+      <c r="D207" s="23"/>
+      <c r="E207" s="23"/>
+      <c r="F207" s="23"/>
+      <c r="G207" s="24"/>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
@@ -5535,26 +5535,26 @@
       <c r="G220" s="2"/>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A221" s="19" t="s">
+      <c r="A221" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B221" s="20"/>
-      <c r="C221" s="20"/>
-      <c r="D221" s="20"/>
-      <c r="E221" s="20"/>
-      <c r="F221" s="20"/>
-      <c r="G221" s="21"/>
+      <c r="B221" s="17"/>
+      <c r="C221" s="17"/>
+      <c r="D221" s="17"/>
+      <c r="E221" s="17"/>
+      <c r="F221" s="17"/>
+      <c r="G221" s="18"/>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A222" s="15" t="s">
+      <c r="A222" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B222" s="16"/>
-      <c r="C222" s="16"/>
-      <c r="D222" s="16"/>
-      <c r="E222" s="16"/>
-      <c r="F222" s="16"/>
-      <c r="G222" s="17"/>
+      <c r="B222" s="23"/>
+      <c r="C222" s="23"/>
+      <c r="D222" s="23"/>
+      <c r="E222" s="23"/>
+      <c r="F222" s="23"/>
+      <c r="G222" s="24"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
@@ -5703,26 +5703,26 @@
       <c r="G230" s="2"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="19" t="s">
+      <c r="A231" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="B231" s="20"/>
-      <c r="C231" s="20"/>
-      <c r="D231" s="20"/>
-      <c r="E231" s="20"/>
-      <c r="F231" s="20"/>
-      <c r="G231" s="21"/>
+      <c r="B231" s="17"/>
+      <c r="C231" s="17"/>
+      <c r="D231" s="17"/>
+      <c r="E231" s="17"/>
+      <c r="F231" s="17"/>
+      <c r="G231" s="18"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232" s="15" t="s">
+      <c r="A232" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B232" s="16"/>
-      <c r="C232" s="16"/>
-      <c r="D232" s="16"/>
-      <c r="E232" s="16"/>
-      <c r="F232" s="16"/>
-      <c r="G232" s="17"/>
+      <c r="B232" s="23"/>
+      <c r="C232" s="23"/>
+      <c r="D232" s="23"/>
+      <c r="E232" s="23"/>
+      <c r="F232" s="23"/>
+      <c r="G232" s="24"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
@@ -5795,26 +5795,26 @@
       <c r="G236" s="2"/>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A237" s="19" t="s">
+      <c r="A237" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B237" s="20"/>
-      <c r="C237" s="20"/>
-      <c r="D237" s="20"/>
-      <c r="E237" s="20"/>
-      <c r="F237" s="20"/>
-      <c r="G237" s="21"/>
+      <c r="B237" s="17"/>
+      <c r="C237" s="17"/>
+      <c r="D237" s="17"/>
+      <c r="E237" s="17"/>
+      <c r="F237" s="17"/>
+      <c r="G237" s="18"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A238" s="15" t="s">
+      <c r="A238" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B238" s="16"/>
-      <c r="C238" s="16"/>
-      <c r="D238" s="16"/>
-      <c r="E238" s="16"/>
-      <c r="F238" s="16"/>
-      <c r="G238" s="17"/>
+      <c r="B238" s="23"/>
+      <c r="C238" s="23"/>
+      <c r="D238" s="23"/>
+      <c r="E238" s="23"/>
+      <c r="F238" s="23"/>
+      <c r="G238" s="24"/>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
@@ -5906,26 +5906,26 @@
       <c r="G243" s="2"/>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="19" t="s">
+      <c r="A244" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B244" s="20"/>
-      <c r="C244" s="20"/>
-      <c r="D244" s="20"/>
-      <c r="E244" s="20"/>
-      <c r="F244" s="20"/>
-      <c r="G244" s="21"/>
+      <c r="B244" s="17"/>
+      <c r="C244" s="17"/>
+      <c r="D244" s="17"/>
+      <c r="E244" s="17"/>
+      <c r="F244" s="17"/>
+      <c r="G244" s="18"/>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" s="15" t="s">
+      <c r="A245" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B245" s="16"/>
-      <c r="C245" s="16"/>
-      <c r="D245" s="16"/>
-      <c r="E245" s="16"/>
-      <c r="F245" s="16"/>
-      <c r="G245" s="17"/>
+      <c r="B245" s="23"/>
+      <c r="C245" s="23"/>
+      <c r="D245" s="23"/>
+      <c r="E245" s="23"/>
+      <c r="F245" s="23"/>
+      <c r="G245" s="24"/>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
@@ -6057,26 +6057,26 @@
       <c r="G252" s="2"/>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="19" t="s">
+      <c r="A253" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B253" s="20"/>
-      <c r="C253" s="20"/>
-      <c r="D253" s="20"/>
-      <c r="E253" s="20"/>
-      <c r="F253" s="20"/>
-      <c r="G253" s="21"/>
+      <c r="B253" s="17"/>
+      <c r="C253" s="17"/>
+      <c r="D253" s="17"/>
+      <c r="E253" s="17"/>
+      <c r="F253" s="17"/>
+      <c r="G253" s="18"/>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="15" t="s">
+      <c r="A254" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B254" s="16"/>
-      <c r="C254" s="16"/>
-      <c r="D254" s="16"/>
-      <c r="E254" s="16"/>
-      <c r="F254" s="16"/>
-      <c r="G254" s="17"/>
+      <c r="B254" s="23"/>
+      <c r="C254" s="23"/>
+      <c r="D254" s="23"/>
+      <c r="E254" s="23"/>
+      <c r="F254" s="23"/>
+      <c r="G254" s="24"/>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
@@ -6187,26 +6187,26 @@
       <c r="G260" s="2"/>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="19" t="s">
+      <c r="A261" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B261" s="20"/>
-      <c r="C261" s="20"/>
-      <c r="D261" s="20"/>
-      <c r="E261" s="20"/>
-      <c r="F261" s="20"/>
-      <c r="G261" s="21"/>
+      <c r="B261" s="17"/>
+      <c r="C261" s="17"/>
+      <c r="D261" s="17"/>
+      <c r="E261" s="17"/>
+      <c r="F261" s="17"/>
+      <c r="G261" s="18"/>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="15" t="s">
+      <c r="A262" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B262" s="16"/>
-      <c r="C262" s="16"/>
-      <c r="D262" s="16"/>
-      <c r="E262" s="16"/>
-      <c r="F262" s="16"/>
-      <c r="G262" s="17"/>
+      <c r="B262" s="23"/>
+      <c r="C262" s="23"/>
+      <c r="D262" s="23"/>
+      <c r="E262" s="23"/>
+      <c r="F262" s="23"/>
+      <c r="G262" s="24"/>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
@@ -6336,26 +6336,26 @@
       <c r="G269" s="2"/>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" s="19" t="s">
+      <c r="A270" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B270" s="20"/>
-      <c r="C270" s="20"/>
-      <c r="D270" s="20"/>
-      <c r="E270" s="20"/>
-      <c r="F270" s="20"/>
-      <c r="G270" s="21"/>
+      <c r="B270" s="17"/>
+      <c r="C270" s="17"/>
+      <c r="D270" s="17"/>
+      <c r="E270" s="17"/>
+      <c r="F270" s="17"/>
+      <c r="G270" s="18"/>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A271" s="15" t="s">
+      <c r="A271" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B271" s="16"/>
-      <c r="C271" s="16"/>
-      <c r="D271" s="16"/>
-      <c r="E271" s="16"/>
-      <c r="F271" s="16"/>
-      <c r="G271" s="17"/>
+      <c r="B271" s="23"/>
+      <c r="C271" s="23"/>
+      <c r="D271" s="23"/>
+      <c r="E271" s="23"/>
+      <c r="F271" s="23"/>
+      <c r="G271" s="24"/>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
@@ -6468,26 +6468,26 @@
       <c r="G277" s="2"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="19" t="s">
+      <c r="A278" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="B278" s="20"/>
-      <c r="C278" s="20"/>
-      <c r="D278" s="20"/>
-      <c r="E278" s="20"/>
-      <c r="F278" s="20"/>
-      <c r="G278" s="21"/>
+      <c r="B278" s="17"/>
+      <c r="C278" s="17"/>
+      <c r="D278" s="17"/>
+      <c r="E278" s="17"/>
+      <c r="F278" s="17"/>
+      <c r="G278" s="18"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" s="15" t="s">
+      <c r="A279" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B279" s="16"/>
-      <c r="C279" s="16"/>
-      <c r="D279" s="16"/>
-      <c r="E279" s="16"/>
-      <c r="F279" s="16"/>
-      <c r="G279" s="17"/>
+      <c r="B279" s="23"/>
+      <c r="C279" s="23"/>
+      <c r="D279" s="23"/>
+      <c r="E279" s="23"/>
+      <c r="F279" s="23"/>
+      <c r="G279" s="24"/>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
@@ -6598,26 +6598,26 @@
       <c r="G285" s="2"/>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="19" t="s">
+      <c r="A286" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B286" s="20"/>
-      <c r="C286" s="20"/>
-      <c r="D286" s="20"/>
-      <c r="E286" s="20"/>
-      <c r="F286" s="20"/>
-      <c r="G286" s="21"/>
+      <c r="B286" s="17"/>
+      <c r="C286" s="17"/>
+      <c r="D286" s="17"/>
+      <c r="E286" s="17"/>
+      <c r="F286" s="17"/>
+      <c r="G286" s="18"/>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="15" t="s">
+      <c r="A287" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B287" s="16"/>
-      <c r="C287" s="16"/>
-      <c r="D287" s="16"/>
-      <c r="E287" s="16"/>
-      <c r="F287" s="16"/>
-      <c r="G287" s="17"/>
+      <c r="B287" s="23"/>
+      <c r="C287" s="23"/>
+      <c r="D287" s="23"/>
+      <c r="E287" s="23"/>
+      <c r="F287" s="23"/>
+      <c r="G287" s="24"/>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
@@ -6937,26 +6937,26 @@
       <c r="G304" s="2"/>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="19" t="s">
+      <c r="A305" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="B305" s="20"/>
-      <c r="C305" s="20"/>
-      <c r="D305" s="20"/>
-      <c r="E305" s="20"/>
-      <c r="F305" s="20"/>
-      <c r="G305" s="21"/>
+      <c r="B305" s="17"/>
+      <c r="C305" s="17"/>
+      <c r="D305" s="17"/>
+      <c r="E305" s="17"/>
+      <c r="F305" s="17"/>
+      <c r="G305" s="18"/>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306" s="15" t="s">
+      <c r="A306" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B306" s="16"/>
-      <c r="C306" s="16"/>
-      <c r="D306" s="16"/>
-      <c r="E306" s="16"/>
-      <c r="F306" s="16"/>
-      <c r="G306" s="17"/>
+      <c r="B306" s="23"/>
+      <c r="C306" s="23"/>
+      <c r="D306" s="23"/>
+      <c r="E306" s="23"/>
+      <c r="F306" s="23"/>
+      <c r="G306" s="24"/>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
@@ -7071,26 +7071,26 @@
       <c r="G312" s="2"/>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A313" s="19" t="s">
+      <c r="A313" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="B313" s="20"/>
-      <c r="C313" s="20"/>
-      <c r="D313" s="20"/>
-      <c r="E313" s="20"/>
-      <c r="F313" s="20"/>
-      <c r="G313" s="21"/>
+      <c r="B313" s="17"/>
+      <c r="C313" s="17"/>
+      <c r="D313" s="17"/>
+      <c r="E313" s="17"/>
+      <c r="F313" s="17"/>
+      <c r="G313" s="18"/>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A314" s="15" t="s">
+      <c r="A314" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B314" s="16"/>
-      <c r="C314" s="16"/>
-      <c r="D314" s="16"/>
-      <c r="E314" s="16"/>
-      <c r="F314" s="16"/>
-      <c r="G314" s="17"/>
+      <c r="B314" s="23"/>
+      <c r="C314" s="23"/>
+      <c r="D314" s="23"/>
+      <c r="E314" s="23"/>
+      <c r="F314" s="23"/>
+      <c r="G314" s="24"/>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
@@ -7163,26 +7163,26 @@
       <c r="G318" s="2"/>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A319" s="19" t="s">
+      <c r="A319" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="B319" s="20"/>
-      <c r="C319" s="20"/>
-      <c r="D319" s="20"/>
-      <c r="E319" s="20"/>
-      <c r="F319" s="20"/>
-      <c r="G319" s="21"/>
+      <c r="B319" s="17"/>
+      <c r="C319" s="17"/>
+      <c r="D319" s="17"/>
+      <c r="E319" s="17"/>
+      <c r="F319" s="17"/>
+      <c r="G319" s="18"/>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A320" s="15" t="s">
+      <c r="A320" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B320" s="16"/>
-      <c r="C320" s="16"/>
-      <c r="D320" s="16"/>
-      <c r="E320" s="16"/>
-      <c r="F320" s="16"/>
-      <c r="G320" s="17"/>
+      <c r="B320" s="23"/>
+      <c r="C320" s="23"/>
+      <c r="D320" s="23"/>
+      <c r="E320" s="23"/>
+      <c r="F320" s="23"/>
+      <c r="G320" s="24"/>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
@@ -7314,26 +7314,26 @@
       <c r="G327" s="2"/>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A328" s="19" t="s">
+      <c r="A328" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="B328" s="20"/>
-      <c r="C328" s="20"/>
-      <c r="D328" s="20"/>
-      <c r="E328" s="20"/>
-      <c r="F328" s="20"/>
-      <c r="G328" s="21"/>
+      <c r="B328" s="17"/>
+      <c r="C328" s="17"/>
+      <c r="D328" s="17"/>
+      <c r="E328" s="17"/>
+      <c r="F328" s="17"/>
+      <c r="G328" s="18"/>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A329" s="15" t="s">
+      <c r="A329" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B329" s="16"/>
-      <c r="C329" s="16"/>
-      <c r="D329" s="16"/>
-      <c r="E329" s="16"/>
-      <c r="F329" s="16"/>
-      <c r="G329" s="17"/>
+      <c r="B329" s="23"/>
+      <c r="C329" s="23"/>
+      <c r="D329" s="23"/>
+      <c r="E329" s="23"/>
+      <c r="F329" s="23"/>
+      <c r="G329" s="24"/>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="4" t="s">
@@ -7406,26 +7406,26 @@
       <c r="G333" s="2"/>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A334" s="19" t="s">
+      <c r="A334" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B334" s="20"/>
-      <c r="C334" s="20"/>
-      <c r="D334" s="20"/>
-      <c r="E334" s="20"/>
-      <c r="F334" s="20"/>
-      <c r="G334" s="21"/>
+      <c r="B334" s="17"/>
+      <c r="C334" s="17"/>
+      <c r="D334" s="17"/>
+      <c r="E334" s="17"/>
+      <c r="F334" s="17"/>
+      <c r="G334" s="18"/>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A335" s="15" t="s">
+      <c r="A335" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B335" s="16"/>
-      <c r="C335" s="16"/>
-      <c r="D335" s="16"/>
-      <c r="E335" s="16"/>
-      <c r="F335" s="16"/>
-      <c r="G335" s="17"/>
+      <c r="B335" s="23"/>
+      <c r="C335" s="23"/>
+      <c r="D335" s="23"/>
+      <c r="E335" s="23"/>
+      <c r="F335" s="23"/>
+      <c r="G335" s="24"/>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="4" t="s">
@@ -7578,26 +7578,26 @@
       <c r="G343" s="2"/>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A344" s="19" t="s">
+      <c r="A344" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B344" s="20"/>
-      <c r="C344" s="20"/>
-      <c r="D344" s="20"/>
-      <c r="E344" s="20"/>
-      <c r="F344" s="20"/>
-      <c r="G344" s="21"/>
+      <c r="B344" s="17"/>
+      <c r="C344" s="17"/>
+      <c r="D344" s="17"/>
+      <c r="E344" s="17"/>
+      <c r="F344" s="17"/>
+      <c r="G344" s="18"/>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A345" s="15" t="s">
+      <c r="A345" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B345" s="16"/>
-      <c r="C345" s="16"/>
-      <c r="D345" s="16"/>
-      <c r="E345" s="16"/>
-      <c r="F345" s="16"/>
-      <c r="G345" s="17"/>
+      <c r="B345" s="23"/>
+      <c r="C345" s="23"/>
+      <c r="D345" s="23"/>
+      <c r="E345" s="23"/>
+      <c r="F345" s="23"/>
+      <c r="G345" s="24"/>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="4" t="s">
@@ -7710,26 +7710,26 @@
       <c r="G351" s="2"/>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A352" s="19" t="s">
+      <c r="A352" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B352" s="20"/>
-      <c r="C352" s="20"/>
-      <c r="D352" s="20"/>
-      <c r="E352" s="20"/>
-      <c r="F352" s="20"/>
-      <c r="G352" s="21"/>
+      <c r="B352" s="17"/>
+      <c r="C352" s="17"/>
+      <c r="D352" s="17"/>
+      <c r="E352" s="17"/>
+      <c r="F352" s="17"/>
+      <c r="G352" s="18"/>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A353" s="15" t="s">
+      <c r="A353" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B353" s="16"/>
-      <c r="C353" s="16"/>
-      <c r="D353" s="16"/>
-      <c r="E353" s="16"/>
-      <c r="F353" s="16"/>
-      <c r="G353" s="17"/>
+      <c r="B353" s="23"/>
+      <c r="C353" s="23"/>
+      <c r="D353" s="23"/>
+      <c r="E353" s="23"/>
+      <c r="F353" s="23"/>
+      <c r="G353" s="24"/>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="4" t="s">
@@ -7880,26 +7880,26 @@
       <c r="G361" s="2"/>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362" s="19" t="s">
+      <c r="A362" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B362" s="20"/>
-      <c r="C362" s="20"/>
-      <c r="D362" s="20"/>
-      <c r="E362" s="20"/>
-      <c r="F362" s="20"/>
-      <c r="G362" s="21"/>
+      <c r="B362" s="17"/>
+      <c r="C362" s="17"/>
+      <c r="D362" s="17"/>
+      <c r="E362" s="17"/>
+      <c r="F362" s="17"/>
+      <c r="G362" s="18"/>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A363" s="15" t="s">
+      <c r="A363" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B363" s="16"/>
-      <c r="C363" s="16"/>
-      <c r="D363" s="16"/>
-      <c r="E363" s="16"/>
-      <c r="F363" s="16"/>
-      <c r="G363" s="17"/>
+      <c r="B363" s="23"/>
+      <c r="C363" s="23"/>
+      <c r="D363" s="23"/>
+      <c r="E363" s="23"/>
+      <c r="F363" s="23"/>
+      <c r="G363" s="24"/>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="4" t="s">
@@ -8012,26 +8012,26 @@
       <c r="G369" s="2"/>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A370" s="23" t="s">
+      <c r="A370" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="B370" s="24"/>
-      <c r="C370" s="24"/>
-      <c r="D370" s="24"/>
-      <c r="E370" s="24"/>
-      <c r="F370" s="24"/>
-      <c r="G370" s="25"/>
+      <c r="B370" s="20"/>
+      <c r="C370" s="20"/>
+      <c r="D370" s="20"/>
+      <c r="E370" s="20"/>
+      <c r="F370" s="20"/>
+      <c r="G370" s="21"/>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A371" s="15" t="s">
+      <c r="A371" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B371" s="16"/>
-      <c r="C371" s="16"/>
-      <c r="D371" s="16"/>
-      <c r="E371" s="16"/>
-      <c r="F371" s="16"/>
-      <c r="G371" s="17"/>
+      <c r="B371" s="23"/>
+      <c r="C371" s="23"/>
+      <c r="D371" s="23"/>
+      <c r="E371" s="23"/>
+      <c r="F371" s="23"/>
+      <c r="G371" s="24"/>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
@@ -8123,26 +8123,26 @@
       <c r="G376" s="2"/>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A377" s="23" t="s">
+      <c r="A377" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B377" s="24"/>
-      <c r="C377" s="24"/>
-      <c r="D377" s="24"/>
-      <c r="E377" s="24"/>
-      <c r="F377" s="24"/>
-      <c r="G377" s="25"/>
+      <c r="B377" s="20"/>
+      <c r="C377" s="20"/>
+      <c r="D377" s="20"/>
+      <c r="E377" s="20"/>
+      <c r="F377" s="20"/>
+      <c r="G377" s="21"/>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A378" s="15" t="s">
+      <c r="A378" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B378" s="16"/>
-      <c r="C378" s="16"/>
-      <c r="D378" s="16"/>
-      <c r="E378" s="16"/>
-      <c r="F378" s="16"/>
-      <c r="G378" s="17"/>
+      <c r="B378" s="23"/>
+      <c r="C378" s="23"/>
+      <c r="D378" s="23"/>
+      <c r="E378" s="23"/>
+      <c r="F378" s="23"/>
+      <c r="G378" s="24"/>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="4" t="s">
@@ -8255,26 +8255,26 @@
       <c r="G384" s="2"/>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A385" s="19" t="s">
+      <c r="A385" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B385" s="20"/>
-      <c r="C385" s="20"/>
-      <c r="D385" s="20"/>
-      <c r="E385" s="20"/>
-      <c r="F385" s="20"/>
-      <c r="G385" s="21"/>
+      <c r="B385" s="17"/>
+      <c r="C385" s="17"/>
+      <c r="D385" s="17"/>
+      <c r="E385" s="17"/>
+      <c r="F385" s="17"/>
+      <c r="G385" s="18"/>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A386" s="15" t="s">
+      <c r="A386" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B386" s="16"/>
-      <c r="C386" s="16"/>
-      <c r="D386" s="16"/>
-      <c r="E386" s="16"/>
-      <c r="F386" s="16"/>
-      <c r="G386" s="17"/>
+      <c r="B386" s="23"/>
+      <c r="C386" s="23"/>
+      <c r="D386" s="23"/>
+      <c r="E386" s="23"/>
+      <c r="F386" s="23"/>
+      <c r="G386" s="24"/>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="4" t="s">
@@ -8366,26 +8366,26 @@
       <c r="G391" s="2"/>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A392" s="19" t="s">
+      <c r="A392" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="B392" s="20"/>
-      <c r="C392" s="20"/>
-      <c r="D392" s="20"/>
-      <c r="E392" s="20"/>
-      <c r="F392" s="20"/>
-      <c r="G392" s="21"/>
+      <c r="B392" s="17"/>
+      <c r="C392" s="17"/>
+      <c r="D392" s="17"/>
+      <c r="E392" s="17"/>
+      <c r="F392" s="17"/>
+      <c r="G392" s="18"/>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A393" s="15" t="s">
+      <c r="A393" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B393" s="16"/>
-      <c r="C393" s="16"/>
-      <c r="D393" s="16"/>
-      <c r="E393" s="16"/>
-      <c r="F393" s="16"/>
-      <c r="G393" s="17"/>
+      <c r="B393" s="23"/>
+      <c r="C393" s="23"/>
+      <c r="D393" s="23"/>
+      <c r="E393" s="23"/>
+      <c r="F393" s="23"/>
+      <c r="G393" s="24"/>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="4" t="s">
@@ -8498,26 +8498,26 @@
       <c r="G399" s="2"/>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A400" s="19" t="s">
+      <c r="A400" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B400" s="20"/>
-      <c r="C400" s="20"/>
-      <c r="D400" s="20"/>
-      <c r="E400" s="20"/>
-      <c r="F400" s="20"/>
-      <c r="G400" s="21"/>
+      <c r="B400" s="17"/>
+      <c r="C400" s="17"/>
+      <c r="D400" s="17"/>
+      <c r="E400" s="17"/>
+      <c r="F400" s="17"/>
+      <c r="G400" s="18"/>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A401" s="15" t="s">
+      <c r="A401" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B401" s="16"/>
-      <c r="C401" s="16"/>
-      <c r="D401" s="16"/>
-      <c r="E401" s="16"/>
-      <c r="F401" s="16"/>
-      <c r="G401" s="17"/>
+      <c r="B401" s="23"/>
+      <c r="C401" s="23"/>
+      <c r="D401" s="23"/>
+      <c r="E401" s="23"/>
+      <c r="F401" s="23"/>
+      <c r="G401" s="24"/>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="4" t="s">
@@ -8590,26 +8590,26 @@
       <c r="G405" s="2"/>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A406" s="19" t="s">
+      <c r="A406" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B406" s="20"/>
-      <c r="C406" s="20"/>
-      <c r="D406" s="20"/>
-      <c r="E406" s="20"/>
-      <c r="F406" s="20"/>
-      <c r="G406" s="21"/>
+      <c r="B406" s="17"/>
+      <c r="C406" s="17"/>
+      <c r="D406" s="17"/>
+      <c r="E406" s="17"/>
+      <c r="F406" s="17"/>
+      <c r="G406" s="18"/>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A407" s="15" t="s">
+      <c r="A407" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B407" s="16"/>
-      <c r="C407" s="16"/>
-      <c r="D407" s="16"/>
-      <c r="E407" s="16"/>
-      <c r="F407" s="16"/>
-      <c r="G407" s="17"/>
+      <c r="B407" s="23"/>
+      <c r="C407" s="23"/>
+      <c r="D407" s="23"/>
+      <c r="E407" s="23"/>
+      <c r="F407" s="23"/>
+      <c r="G407" s="24"/>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="4" t="s">
@@ -8701,26 +8701,26 @@
       <c r="G412" s="2"/>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A413" s="19" t="s">
+      <c r="A413" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B413" s="20"/>
-      <c r="C413" s="20"/>
-      <c r="D413" s="20"/>
-      <c r="E413" s="20"/>
-      <c r="F413" s="20"/>
-      <c r="G413" s="21"/>
+      <c r="B413" s="17"/>
+      <c r="C413" s="17"/>
+      <c r="D413" s="17"/>
+      <c r="E413" s="17"/>
+      <c r="F413" s="17"/>
+      <c r="G413" s="18"/>
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A414" s="15" t="s">
+      <c r="A414" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B414" s="16"/>
-      <c r="C414" s="16"/>
-      <c r="D414" s="16"/>
-      <c r="E414" s="16"/>
-      <c r="F414" s="16"/>
-      <c r="G414" s="17"/>
+      <c r="B414" s="23"/>
+      <c r="C414" s="23"/>
+      <c r="D414" s="23"/>
+      <c r="E414" s="23"/>
+      <c r="F414" s="23"/>
+      <c r="G414" s="24"/>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="4" t="s">
@@ -8793,26 +8793,26 @@
       <c r="G418" s="2"/>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A419" s="19" t="s">
+      <c r="A419" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B419" s="20"/>
-      <c r="C419" s="20"/>
-      <c r="D419" s="20"/>
-      <c r="E419" s="20"/>
-      <c r="F419" s="20"/>
-      <c r="G419" s="21"/>
+      <c r="B419" s="17"/>
+      <c r="C419" s="17"/>
+      <c r="D419" s="17"/>
+      <c r="E419" s="17"/>
+      <c r="F419" s="17"/>
+      <c r="G419" s="18"/>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A420" s="15" t="s">
+      <c r="A420" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B420" s="16"/>
-      <c r="C420" s="16"/>
-      <c r="D420" s="16"/>
-      <c r="E420" s="16"/>
-      <c r="F420" s="16"/>
-      <c r="G420" s="17"/>
+      <c r="B420" s="23"/>
+      <c r="C420" s="23"/>
+      <c r="D420" s="23"/>
+      <c r="E420" s="23"/>
+      <c r="F420" s="23"/>
+      <c r="G420" s="24"/>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="4" t="s">
@@ -8925,26 +8925,26 @@
       <c r="G426" s="2"/>
     </row>
     <row r="427" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A427" s="19" t="s">
+      <c r="A427" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="B427" s="20"/>
-      <c r="C427" s="20"/>
-      <c r="D427" s="20"/>
-      <c r="E427" s="20"/>
-      <c r="F427" s="20"/>
-      <c r="G427" s="21"/>
+      <c r="B427" s="17"/>
+      <c r="C427" s="17"/>
+      <c r="D427" s="17"/>
+      <c r="E427" s="17"/>
+      <c r="F427" s="17"/>
+      <c r="G427" s="18"/>
     </row>
     <row r="428" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A428" s="15" t="s">
+      <c r="A428" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B428" s="16"/>
-      <c r="C428" s="16"/>
-      <c r="D428" s="16"/>
-      <c r="E428" s="16"/>
-      <c r="F428" s="16"/>
-      <c r="G428" s="17"/>
+      <c r="B428" s="23"/>
+      <c r="C428" s="23"/>
+      <c r="D428" s="23"/>
+      <c r="E428" s="23"/>
+      <c r="F428" s="23"/>
+      <c r="G428" s="24"/>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" s="4" t="s">
@@ -9057,26 +9057,26 @@
       <c r="G434" s="2"/>
     </row>
     <row r="435" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A435" s="19" t="s">
+      <c r="A435" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B435" s="20"/>
-      <c r="C435" s="20"/>
-      <c r="D435" s="20"/>
-      <c r="E435" s="20"/>
-      <c r="F435" s="20"/>
-      <c r="G435" s="21"/>
+      <c r="B435" s="17"/>
+      <c r="C435" s="17"/>
+      <c r="D435" s="17"/>
+      <c r="E435" s="17"/>
+      <c r="F435" s="17"/>
+      <c r="G435" s="18"/>
     </row>
     <row r="436" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A436" s="15" t="s">
+      <c r="A436" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B436" s="16"/>
-      <c r="C436" s="16"/>
-      <c r="D436" s="16"/>
-      <c r="E436" s="16"/>
-      <c r="F436" s="16"/>
-      <c r="G436" s="17"/>
+      <c r="B436" s="23"/>
+      <c r="C436" s="23"/>
+      <c r="D436" s="23"/>
+      <c r="E436" s="23"/>
+      <c r="F436" s="23"/>
+      <c r="G436" s="24"/>
     </row>
     <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" s="4" t="s">
@@ -9140,26 +9140,26 @@
       <c r="G439" s="5"/>
     </row>
     <row r="441" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A441" s="18" t="s">
+      <c r="A441" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="B441" s="22"/>
-      <c r="C441" s="22"/>
-      <c r="D441" s="22"/>
-      <c r="E441" s="22"/>
-      <c r="F441" s="22"/>
-      <c r="G441" s="22"/>
+      <c r="B441" s="15"/>
+      <c r="C441" s="15"/>
+      <c r="D441" s="15"/>
+      <c r="E441" s="15"/>
+      <c r="F441" s="15"/>
+      <c r="G441" s="15"/>
     </row>
     <row r="442" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A442" s="18" t="s">
+      <c r="A442" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B442" s="18"/>
-      <c r="C442" s="18"/>
-      <c r="D442" s="18"/>
-      <c r="E442" s="18"/>
-      <c r="F442" s="18"/>
-      <c r="G442" s="18"/>
+      <c r="B442" s="14"/>
+      <c r="C442" s="14"/>
+      <c r="D442" s="14"/>
+      <c r="E442" s="14"/>
+      <c r="F442" s="14"/>
+      <c r="G442" s="14"/>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A443" s="8" t="s">
@@ -9320,26 +9320,26 @@
       <c r="G450" s="10"/>
     </row>
     <row r="452" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A452" s="18" t="s">
+      <c r="A452" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="B452" s="22"/>
-      <c r="C452" s="22"/>
-      <c r="D452" s="22"/>
-      <c r="E452" s="22"/>
-      <c r="F452" s="22"/>
-      <c r="G452" s="22"/>
+      <c r="B452" s="15"/>
+      <c r="C452" s="15"/>
+      <c r="D452" s="15"/>
+      <c r="E452" s="15"/>
+      <c r="F452" s="15"/>
+      <c r="G452" s="15"/>
     </row>
     <row r="453" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A453" s="18" t="s">
+      <c r="A453" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B453" s="18"/>
-      <c r="C453" s="18"/>
-      <c r="D453" s="18"/>
-      <c r="E453" s="18"/>
-      <c r="F453" s="18"/>
-      <c r="G453" s="18"/>
+      <c r="B453" s="14"/>
+      <c r="C453" s="14"/>
+      <c r="D453" s="14"/>
+      <c r="E453" s="14"/>
+      <c r="F453" s="14"/>
+      <c r="G453" s="14"/>
     </row>
     <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="8" t="s">
@@ -9459,26 +9459,26 @@
       <c r="G460" s="13"/>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A461" s="18" t="s">
+      <c r="A461" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="B461" s="22"/>
-      <c r="C461" s="22"/>
-      <c r="D461" s="22"/>
-      <c r="E461" s="22"/>
-      <c r="F461" s="22"/>
-      <c r="G461" s="22"/>
+      <c r="B461" s="15"/>
+      <c r="C461" s="15"/>
+      <c r="D461" s="15"/>
+      <c r="E461" s="15"/>
+      <c r="F461" s="15"/>
+      <c r="G461" s="15"/>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A462" s="19" t="s">
+      <c r="A462" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B462" s="20"/>
-      <c r="C462" s="20"/>
-      <c r="D462" s="20"/>
-      <c r="E462" s="20"/>
-      <c r="F462" s="20"/>
-      <c r="G462" s="21"/>
+      <c r="B462" s="17"/>
+      <c r="C462" s="17"/>
+      <c r="D462" s="17"/>
+      <c r="E462" s="17"/>
+      <c r="F462" s="17"/>
+      <c r="G462" s="18"/>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="8" t="s">
@@ -9561,44 +9561,54 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="A461:G461"/>
-    <mergeCell ref="A462:G462"/>
-    <mergeCell ref="A452:G452"/>
-    <mergeCell ref="A453:G453"/>
-    <mergeCell ref="A413:G413"/>
-    <mergeCell ref="A435:G435"/>
-    <mergeCell ref="A419:G419"/>
-    <mergeCell ref="A427:G427"/>
-    <mergeCell ref="A370:G370"/>
-    <mergeCell ref="A377:G377"/>
-    <mergeCell ref="A385:G385"/>
-    <mergeCell ref="A392:G392"/>
-    <mergeCell ref="A400:G400"/>
-    <mergeCell ref="A414:G414"/>
-    <mergeCell ref="A420:G420"/>
-    <mergeCell ref="A428:G428"/>
-    <mergeCell ref="A441:G441"/>
-    <mergeCell ref="A442:G442"/>
-    <mergeCell ref="A200:G200"/>
-    <mergeCell ref="A261:G261"/>
-    <mergeCell ref="A270:G270"/>
-    <mergeCell ref="A278:G278"/>
-    <mergeCell ref="A305:G305"/>
-    <mergeCell ref="A334:G334"/>
-    <mergeCell ref="A328:G328"/>
-    <mergeCell ref="A313:G313"/>
-    <mergeCell ref="A319:G319"/>
-    <mergeCell ref="A206:G206"/>
-    <mergeCell ref="A262:G262"/>
-    <mergeCell ref="A271:G271"/>
-    <mergeCell ref="A279:G279"/>
-    <mergeCell ref="A287:G287"/>
-    <mergeCell ref="A306:G306"/>
-    <mergeCell ref="A314:G314"/>
-    <mergeCell ref="A286:G286"/>
-    <mergeCell ref="A245:G245"/>
-    <mergeCell ref="A254:G254"/>
-    <mergeCell ref="A253:G253"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="A147:G147"/>
+    <mergeCell ref="A153:G153"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A108:G108"/>
+    <mergeCell ref="A114:G114"/>
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A89:G89"/>
+    <mergeCell ref="A137:G137"/>
+    <mergeCell ref="A129:G129"/>
+    <mergeCell ref="A123:G123"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="A130:G130"/>
+    <mergeCell ref="A436:G436"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A371:G371"/>
+    <mergeCell ref="A378:G378"/>
+    <mergeCell ref="A386:G386"/>
+    <mergeCell ref="A393:G393"/>
+    <mergeCell ref="A401:G401"/>
+    <mergeCell ref="A407:G407"/>
+    <mergeCell ref="A406:G406"/>
+    <mergeCell ref="A320:G320"/>
+    <mergeCell ref="A329:G329"/>
+    <mergeCell ref="A335:G335"/>
+    <mergeCell ref="A345:G345"/>
+    <mergeCell ref="A353:G353"/>
+    <mergeCell ref="A363:G363"/>
+    <mergeCell ref="A344:G344"/>
+    <mergeCell ref="A362:G362"/>
+    <mergeCell ref="A352:G352"/>
+    <mergeCell ref="A107:G107"/>
     <mergeCell ref="A113:G113"/>
     <mergeCell ref="A161:G161"/>
     <mergeCell ref="A146:G146"/>
@@ -9623,54 +9633,44 @@
     <mergeCell ref="A181:G181"/>
     <mergeCell ref="A188:G188"/>
     <mergeCell ref="A194:G194"/>
-    <mergeCell ref="A123:G123"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="A124:G124"/>
-    <mergeCell ref="A130:G130"/>
-    <mergeCell ref="A436:G436"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A371:G371"/>
-    <mergeCell ref="A378:G378"/>
-    <mergeCell ref="A386:G386"/>
-    <mergeCell ref="A393:G393"/>
-    <mergeCell ref="A401:G401"/>
-    <mergeCell ref="A407:G407"/>
-    <mergeCell ref="A406:G406"/>
-    <mergeCell ref="A320:G320"/>
-    <mergeCell ref="A329:G329"/>
-    <mergeCell ref="A335:G335"/>
-    <mergeCell ref="A345:G345"/>
-    <mergeCell ref="A353:G353"/>
-    <mergeCell ref="A363:G363"/>
-    <mergeCell ref="A344:G344"/>
-    <mergeCell ref="A362:G362"/>
-    <mergeCell ref="A352:G352"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="A147:G147"/>
-    <mergeCell ref="A153:G153"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="A114:G114"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A89:G89"/>
-    <mergeCell ref="A137:G137"/>
-    <mergeCell ref="A129:G129"/>
+    <mergeCell ref="A200:G200"/>
+    <mergeCell ref="A261:G261"/>
+    <mergeCell ref="A270:G270"/>
+    <mergeCell ref="A278:G278"/>
+    <mergeCell ref="A305:G305"/>
+    <mergeCell ref="A334:G334"/>
+    <mergeCell ref="A328:G328"/>
+    <mergeCell ref="A313:G313"/>
+    <mergeCell ref="A319:G319"/>
+    <mergeCell ref="A206:G206"/>
+    <mergeCell ref="A262:G262"/>
+    <mergeCell ref="A271:G271"/>
+    <mergeCell ref="A279:G279"/>
+    <mergeCell ref="A287:G287"/>
+    <mergeCell ref="A306:G306"/>
+    <mergeCell ref="A314:G314"/>
+    <mergeCell ref="A286:G286"/>
+    <mergeCell ref="A245:G245"/>
+    <mergeCell ref="A254:G254"/>
+    <mergeCell ref="A253:G253"/>
+    <mergeCell ref="A461:G461"/>
+    <mergeCell ref="A462:G462"/>
+    <mergeCell ref="A452:G452"/>
+    <mergeCell ref="A453:G453"/>
+    <mergeCell ref="A413:G413"/>
+    <mergeCell ref="A435:G435"/>
+    <mergeCell ref="A419:G419"/>
+    <mergeCell ref="A427:G427"/>
+    <mergeCell ref="A370:G370"/>
+    <mergeCell ref="A377:G377"/>
+    <mergeCell ref="A385:G385"/>
+    <mergeCell ref="A392:G392"/>
+    <mergeCell ref="A400:G400"/>
+    <mergeCell ref="A414:G414"/>
+    <mergeCell ref="A420:G420"/>
+    <mergeCell ref="A428:G428"/>
+    <mergeCell ref="A441:G441"/>
+    <mergeCell ref="A442:G442"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>